<commit_message>
removed urls and code
</commit_message>
<xml_diff>
--- a/prompt_responses_rated.xlsx
+++ b/prompt_responses_rated.xlsx
@@ -864,7 +864,11 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>[('## Quantum Computing', 'MONEY'), ('quantum', 'ORG'), ('2024', 'DATE'), ('1', 'CARDINAL'), ('Quantum', 'ORG'), ('quantum', 'ORG'), ('Rigetti', 'LOC'), ('IBM', 'ORG'), ('2', 'CARDINAL'), ('Quantum', 'ORG'), ('Shor', 'PERSON'), ('Grover', 'PERSON'), ('3', 'CARDINAL'), ('New Horizons', 'ORG'), ('Quantum', 'ORG'), ('Quantum', 'ORG'), ('4', 'CARDINAL'), ('quantum', 'ORG'), ('RSA &amp; ECC:*', 'ORG'), ('Quantum', 'ORG'), ('RSA &amp; ECC', 'ORG'), ('PQC', 'ORG'), ('quantum', 'ORG'), ('Quantum', 'ORG'), ('Key Takeaways', 'PERSON'), ('PQC', 'ORG'), ('quantum technologies', 'ORG'), ('PQC', 'ORG'), ('2024', 'DATE'), ('quantum', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE2" t="n">
         <v>100.1532454490662</v>
       </c>
@@ -913,12 +917,20 @@
       <c r="AZ2" t="inlineStr"/>
       <c r="BA2" t="inlineStr"/>
       <c r="BB2" t="inlineStr"/>
-      <c r="BC2" t="inlineStr"/>
-      <c r="BD2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD2" t="n">
+        <v>4262</v>
+      </c>
       <c r="BE2" t="n">
         <v>31</v>
       </c>
-      <c r="BF2" t="inlineStr"/>
+      <c r="BF2" t="n">
+        <v>546</v>
+      </c>
       <c r="BG2" t="n">
         <v>831</v>
       </c>
@@ -1005,7 +1017,11 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>[('2021', 'DATE'), ('2024', 'DATE'), ('the IPCC AR6 Report', 'ORG'), ('2021', 'DATE'), ('1.5', 'CARDINAL'), ('1.5', 'CARDINAL'), ('Arctic', 'LOC'), ('1.5', 'CARDINAL'), ('IPCC', 'ORG'), ('IPCC', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE3" t="n">
         <v>42.30945801734924</v>
       </c>
@@ -1053,13 +1069,25 @@
       <c r="AY3" t="inlineStr"/>
       <c r="AZ3" t="inlineStr"/>
       <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>['https://www.ipcc.ch/.']</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD3" t="n">
+        <v>1691</v>
+      </c>
       <c r="BE3" t="n">
         <v>12</v>
       </c>
-      <c r="BF3" t="inlineStr"/>
+      <c r="BF3" t="n">
+        <v>241</v>
+      </c>
       <c r="BG3" t="n">
         <v>370</v>
       </c>
@@ -1156,7 +1184,11 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>[('#', 'MONEY'), ('Artemis', 'ORG'), ('NASA', 'ORG'), ('Moon', 'PERSON'), ('Artemis', 'ORG'), ('November 2022', 'DATE'), ('Moon', 'PERSON'), ('the Lunar Gateway', 'FAC'), ('first', 'ORDINAL'), ('Gateway', 'PERSON'), ('this year', 'DATE'), ('Starship', 'PERSON'), ('NASA', 'ORG'), ('Space Launch System', 'ORG'), ('Orion', 'ORG'), ('Lockheed Martin', 'PERSON'), ('Artemis', 'ORG'), ('Moon', 'PERSON'), ('first', 'ORDINAL'), ('NASA', 'ORG'), ('Lunar Reconnaissance Orbiter', 'ORG'), ('LRO', 'ORG'), ('Artemis II Mission:*', 'ORG'), ('2024', 'DATE'), ('Moon', 'PERSON'), ('Lunar Gateway Operations:*', 'ORG'), ('first', 'ORDINAL'), ('the Lunar Gateway', 'FAC'), ('the early 2030s', 'DATE'), ('Artemis', 'ORG'), ('Moon', 'PERSON'), ('Artemis', 'ORG'), ('Earth', 'LOC'), ('Moon', 'PERSON'), ('ISRU', 'ORG'), ('Mars', 'LOC'), ('Moon', 'PERSON'), ('Artemis', 'ORG'), ('Moon', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE4" t="n">
         <v>91.65349817276001</v>
       </c>
@@ -1205,12 +1237,20 @@
       <c r="AZ4" t="inlineStr"/>
       <c r="BA4" t="inlineStr"/>
       <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD4" t="n">
+        <v>3896</v>
+      </c>
       <c r="BE4" t="n">
         <v>22</v>
       </c>
-      <c r="BF4" t="inlineStr"/>
+      <c r="BF4" t="n">
+        <v>552</v>
+      </c>
       <c r="BG4" t="n">
         <v>754</v>
       </c>
@@ -1312,7 +1352,11 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>[('CRISPR', 'PERSON'), ('1', 'CARDINAL'), ('CRISPR', 'PERSON'), ('2', 'CARDINAL'), ('Cancer Therapy:*', 'PERSON'), ('CRISPR', 'PERSON'), ('CRISPR', 'PERSON'), ('Gene Silencing', 'PERSON'), ('CRISPR', 'GPE'), ('CFTR', 'ORG'), ('CRISPR technology holds immense', 'ORG'), ('Antimicrobial Resistance:*', 'ORG'), ('Methicillin', 'PERSON'), ('Staphylococcus aureus', 'PERSON'), ('3', 'CARDINAL'), ('CRISPR', 'PERSON'), ('Gene Therapy:*', 'PERSON'), ('4', 'CARDINAL'), ('Challenges and Future Directions', 'ORG'), ('CRISPR', 'GPE'), ('CRISPR', 'PERSON'), ('CRISPR', 'GPE'), ('CRISPR', 'PERSON'), ('CRISPR', 'PERSON'), ('CRISPR', 'PERSON'), ('PubMed', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE5" t="n">
         <v>102.7815997600555</v>
       </c>
@@ -1361,12 +1405,20 @@
       <c r="AZ5" t="inlineStr"/>
       <c r="BA5" t="inlineStr"/>
       <c r="BB5" t="inlineStr"/>
-      <c r="BC5" t="inlineStr"/>
-      <c r="BD5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD5" t="n">
+        <v>4255</v>
+      </c>
       <c r="BE5" t="n">
         <v>31</v>
       </c>
-      <c r="BF5" t="inlineStr"/>
+      <c r="BF5" t="n">
+        <v>539</v>
+      </c>
       <c r="BG5" t="n">
         <v>834</v>
       </c>
@@ -1462,7 +1514,11 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>[('2024', 'DATE'), ('Nobel Prize in Physics', 'WORK_OF_ART'), ('Potential Candidates &amp; Research Areas:*', 'ORG'), ('Quantum Technologies:*', 'ORG'), ('quantum', 'ORG'), ('Fundamental Physics Research:*', 'ORG'), ('the Higgs Boson', 'ORG'), ('Particle Physics:*', 'ORG'), ('Groundbreaking Research:*', 'ORG'), ('Award', 'PERSON'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('Quantum Technologies:*', 'ORG'), ('quantum', 'ORG'), ('3', 'CARDINAL'), ('Neutrino Physics:*', 'ORG'), ('4', 'CARDINAL'), ('Dark Matter &amp; Dark Energy:*', 'ORG'), ('Nobel Prize', 'WORK_OF_ART'), ('The Nobel Prize in Physics', 'WORK_OF_ART'), ('the Swedish Royal Academy of Sciences', 'ORG'), ('Nobelprize.org', 'ORG'), ('the Nobel Prizes', 'WORK_OF_ART'), ('Physics News Outlets:*', 'ORG'), ('Physics', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE6" t="n">
         <v>77.72137665748596</v>
       </c>
@@ -1511,12 +1567,20 @@
       <c r="AZ6" t="inlineStr"/>
       <c r="BA6" t="inlineStr"/>
       <c r="BB6" t="inlineStr"/>
-      <c r="BC6" t="inlineStr"/>
-      <c r="BD6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD6" t="n">
+        <v>3075</v>
+      </c>
       <c r="BE6" t="n">
         <v>23</v>
       </c>
-      <c r="BF6" t="inlineStr"/>
+      <c r="BF6" t="n">
+        <v>411</v>
+      </c>
       <c r="BG6" t="n">
         <v>598</v>
       </c>
@@ -1609,7 +1673,11 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>[('##', 'MONEY'), ('The year 2024', 'DATE'), ('one', 'CARDINAL'), ('International Relations:*', 'ORG'), ('AI', 'ORG'), ('2024', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE7" t="n">
         <v>76.08661985397339</v>
       </c>
@@ -1658,12 +1726,20 @@
       <c r="AZ7" t="inlineStr"/>
       <c r="BA7" t="inlineStr"/>
       <c r="BB7" t="inlineStr"/>
-      <c r="BC7" t="inlineStr"/>
-      <c r="BD7" t="inlineStr"/>
+      <c r="BC7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD7" t="n">
+        <v>3574</v>
+      </c>
       <c r="BE7" t="n">
         <v>21</v>
       </c>
-      <c r="BF7" t="inlineStr"/>
+      <c r="BF7" t="n">
+        <v>466</v>
+      </c>
       <c r="BG7" t="n">
         <v>629</v>
       </c>
@@ -1762,7 +1838,11 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>[('2024', 'CARDINAL'), ('The coming year', 'DATE'), ('Global Recovery &amp; Rebound', 'ORG'), ('2024', 'DATE'), ('COVID-19', 'ORG'), ('Structural Reforms &amp; Investment:*', 'ORG'), ('Demographic Shifts &amp; Emerging Consumer Markets:*', 'ORG'), ('Geopolitical Uncertainty &amp; Conflict:*', 'ORG'), ('Russia', 'GPE'), ('Fluctuations &amp; Exchange Rate Risks:*', 'ORG'), ('Sustainability &amp; Financial Fragility:*', 'ORG'), ('Asia', 'LOC'), ('Countries', 'LOC'), ('India', 'GPE'), ('China', 'GPE'), ('2024', 'DATE'), ('India', 'GPE'), ('China', 'GPE'), ('Latin America:*', 'LOC'), ('Latin American', 'NORP'), ('recent years', 'DATE'), ('Africa', 'LOC'), ('Africa', 'LOC'), ('India', 'GPE'), ('China', 'GPE'), ('2024', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE8" t="n">
         <v>120.6711721420288</v>
       </c>
@@ -1811,12 +1891,20 @@
       <c r="AZ8" t="inlineStr"/>
       <c r="BA8" t="inlineStr"/>
       <c r="BB8" t="inlineStr"/>
-      <c r="BC8" t="inlineStr"/>
-      <c r="BD8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD8" t="n">
+        <v>5304</v>
+      </c>
       <c r="BE8" t="n">
         <v>30</v>
       </c>
-      <c r="BF8" t="inlineStr"/>
+      <c r="BF8" t="n">
+        <v>686</v>
+      </c>
       <c r="BG8" t="n">
         <v>953</v>
       </c>
@@ -1917,7 +2005,11 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>[('## Fusion Energy', 'MONEY'), ('1.', 'CARDINAL'), ('National Ignition Facility', 'ORG'), ('NIF', 'ORG'), ('Livermore National Laboratory', 'ORG'), ('2023', 'DATE'), ('NIF', 'ORG'), ('Princeton Plasma Physics Laboratory', 'ORG'), ('2', 'CARDINAL'), ('Development of New Technologies:*', 'ORG'), ('Magnetic Confinement Fusion', 'ORG'), ('MCF', 'ORG'), ('Inertial Confinement Fusion', 'ORG'), ('3', 'CARDINAL'), ('Clean &amp; Sustainable:** Fusion', 'ORG'), ('Challenges &amp; Road Ahead:*', 'ORG'), ('Safety &amp; waste management:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE9" t="n">
         <v>83.15560221672058</v>
       </c>
@@ -1966,12 +2058,20 @@
       <c r="AZ9" t="inlineStr"/>
       <c r="BA9" t="inlineStr"/>
       <c r="BB9" t="inlineStr"/>
-      <c r="BC9" t="inlineStr"/>
-      <c r="BD9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD9" t="n">
+        <v>3557</v>
+      </c>
       <c r="BE9" t="n">
         <v>23</v>
       </c>
-      <c r="BF9" t="inlineStr"/>
+      <c r="BF9" t="n">
+        <v>469</v>
+      </c>
       <c r="BG9" t="n">
         <v>693</v>
       </c>
@@ -2088,7 +2188,11 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>[('##', 'MONEY'), ('FeFETs', 'WORK_OF_ART'), ('A Deep Dive\n\nFerroelectric', 'WORK_OF_ART'), ('Key Features &amp; Advantages:*', 'ORG'), ('Feature', 'PRODUCT'), ('Traditional Transistors', 'ORG'), ('FeFETs', 'PERSON'), ('Slow', 'PERSON'), ('Fast', 'PERSON'), ('Power Consumption', 'PRODUCT'), ('Moderate', 'PERSON'), ('Memory', 'PRODUCT'), ('Limited', 'ORG'), ('Advanced Electronics:*', 'ORG'), ('Analog Circuits &amp; Signal Processing:*', 'ORG'), ('2D Materials', 'ORG'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('FeFET', 'NORP'), ('FeFET', 'GPE'), ('FeFETs', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE10" t="n">
         <v>127.3822445869446</v>
       </c>
@@ -2137,12 +2241,20 @@
       <c r="AZ10" t="inlineStr"/>
       <c r="BA10" t="inlineStr"/>
       <c r="BB10" t="inlineStr"/>
-      <c r="BC10" t="inlineStr"/>
-      <c r="BD10" t="inlineStr"/>
+      <c r="BC10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD10" t="n">
+        <v>4692</v>
+      </c>
       <c r="BE10" t="n">
         <v>31</v>
       </c>
-      <c r="BF10" t="inlineStr"/>
+      <c r="BF10" t="n">
+        <v>561</v>
+      </c>
       <c r="BG10" t="n">
         <v>949</v>
       </c>
@@ -2236,7 +2348,11 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>[('##', 'MONEY'), ('Modern Warfare', 'ORG'), ('Moral Agency &amp; Responsibility:*', 'ORG'), ('AWS', 'ORG'), ('Taking a Human Life', 'WORK_OF_ART'), ('AWS', 'ORG'), ('AWS', 'ORG'), ('Potential Societal Impacts:*', 'ORG'), ('Military Doctrine &amp; Strategy:*', 'ORG'), ('AWS', 'ORG'), ('AWS', 'ORG'), ('Uneven Access &amp; Disproportionate Impact:*', 'ORG'), ('AWS', 'ORG'), ('International Treaties &amp; Regulations:*', 'ORG'), ('AWS', 'ORG'), ('The United Nations', 'ORG'), ('AWS', 'ORG'), ('AWS', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE11" t="n">
         <v>84.84045839309692</v>
       </c>
@@ -2285,12 +2401,20 @@
       <c r="AZ11" t="inlineStr"/>
       <c r="BA11" t="inlineStr"/>
       <c r="BB11" t="inlineStr"/>
-      <c r="BC11" t="inlineStr"/>
-      <c r="BD11" t="inlineStr"/>
+      <c r="BC11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD11" t="n">
+        <v>3529</v>
+      </c>
       <c r="BE11" t="n">
         <v>22</v>
       </c>
-      <c r="BF11" t="inlineStr"/>
+      <c r="BF11" t="n">
+        <v>467</v>
+      </c>
       <c r="BG11" t="n">
         <v>661</v>
       </c>
@@ -2390,7 +2514,11 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>[('#', 'MONEY'), ('Cons', 'PERSON'), ('the United States', 'GPE'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('Hazard', 'PERSON'), ('UBI', 'ORG'), ('Stakeholders', 'NORP'), ('UBI', 'GPE'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('Social Experimentation:*', 'ORG'), ('UBI', 'ORG'), ('UBI', 'ORG'), ('US', 'GPE'), ('UBI', 'ORG'), ('US', 'GPE')]</t>
+        </is>
+      </c>
       <c r="AE12" t="n">
         <v>107.5992617607117</v>
       </c>
@@ -2439,12 +2567,20 @@
       <c r="AZ12" t="inlineStr"/>
       <c r="BA12" t="inlineStr"/>
       <c r="BB12" t="inlineStr"/>
-      <c r="BC12" t="inlineStr"/>
-      <c r="BD12" t="inlineStr"/>
+      <c r="BC12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD12" t="n">
+        <v>4735</v>
+      </c>
       <c r="BE12" t="n">
         <v>32</v>
       </c>
-      <c r="BF12" t="inlineStr"/>
+      <c r="BF12" t="n">
+        <v>629</v>
+      </c>
       <c r="BG12" t="n">
         <v>872</v>
       </c>
@@ -2554,7 +2690,11 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>[('US', 'GPE'), ('Massive Energy Demand Surge', 'ORG'), ('Overnight', 'WORK_OF_ART'), ('years', 'DATE'), ('decades', 'DATE'), ('overnight', 'TIME'), ('EV', 'ORG'), ('decade', 'DATE'), ('US', 'GPE'), ('Focus on Public Transportation', 'ORG'), ('metro', 'FAC'), ('overnight', 'TIME'), ('US', 'GPE')]</t>
+        </is>
+      </c>
       <c r="AE13" t="n">
         <v>50.86786246299744</v>
       </c>
@@ -2603,12 +2743,20 @@
       <c r="AZ13" t="inlineStr"/>
       <c r="BA13" t="inlineStr"/>
       <c r="BB13" t="inlineStr"/>
-      <c r="BC13" t="inlineStr"/>
-      <c r="BD13" t="inlineStr"/>
+      <c r="BC13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD13" t="n">
+        <v>3467</v>
+      </c>
       <c r="BE13" t="n">
         <v>24</v>
       </c>
-      <c r="BF13" t="inlineStr"/>
+      <c r="BF13" t="n">
+        <v>459</v>
+      </c>
       <c r="BG13" t="n">
         <v>668</v>
       </c>
@@ -2699,7 +2847,11 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>[('## The River of Consciousness: Stream of', 'MONEY'), ("James Joyce's", 'PERSON'), ('Joyce', 'PERSON'), ('linear', 'ORG'), ('Leopold Bloom', 'PRODUCT'), ('Stephen Dedalus', 'PERSON'), ('Internal Monologues &amp; Dialogue:*', 'ORG'), ('Joyce', 'PERSON'), ('Joyce', 'PERSON'), ('Joyce', 'PERSON'), ('Joyce', 'PERSON'), ('post-World War I Europe', 'EVENT'), ("James Joyce's", 'PERSON'), ('today', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE14" t="n">
         <v>60.74453854560852</v>
       </c>
@@ -2748,12 +2900,20 @@
       <c r="AZ14" t="inlineStr"/>
       <c r="BA14" t="inlineStr"/>
       <c r="BB14" t="inlineStr"/>
-      <c r="BC14" t="inlineStr"/>
-      <c r="BD14" t="inlineStr"/>
+      <c r="BC14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD14" t="n">
+        <v>3914</v>
+      </c>
       <c r="BE14" t="n">
         <v>24</v>
       </c>
-      <c r="BF14" t="inlineStr"/>
+      <c r="BF14" t="n">
+        <v>542</v>
+      </c>
       <c r="BG14" t="n">
         <v>764</v>
       </c>
@@ -2845,7 +3005,11 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>[('## Absurdity', 'MONEY'), ("Samuel Beckett's", 'PERSON'), ('Waiting for Godot', 'WORK_OF_ART'), ("Samuel Beckett's", 'PERSON'), ('Waiting for Godot', 'WORK_OF_ART'), ('post-World War II', 'EVENT'), ('Waiting for Godot', 'WORK_OF_ART'), ('Vladimir', 'PERSON'), ('Estragon', 'ORG'), ('Reflection of Post-War Existentialism:*', 'ORG'), ('Waiting for Godot', 'WORK_OF_ART'), ('World War II', 'EVENT'), ('Trauma', 'PERSON'), ('Vladimir', 'PERSON'), ('Estragon', 'ORG'), ('Waiting for Godot', 'WORK_OF_ART'), ('Vladimir', 'PERSON'), ('Estragon', 'ORG'), ('Waiting for Godot', 'WORK_OF_ART'), ('one', 'CARDINAL'), ('Beckett', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE15" t="n">
         <v>71.35194230079651</v>
       </c>
@@ -2894,12 +3058,20 @@
       <c r="AZ15" t="inlineStr"/>
       <c r="BA15" t="inlineStr"/>
       <c r="BB15" t="inlineStr"/>
-      <c r="BC15" t="inlineStr"/>
-      <c r="BD15" t="inlineStr"/>
+      <c r="BC15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD15" t="n">
+        <v>3789</v>
+      </c>
       <c r="BE15" t="n">
         <v>23</v>
       </c>
-      <c r="BF15" t="inlineStr"/>
+      <c r="BF15" t="n">
+        <v>553</v>
+      </c>
       <c r="BG15" t="n">
         <v>796</v>
       </c>
@@ -2996,7 +3168,11 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>[('##  ', 'MONEY'), ('A Tale of Two Worlds', 'WORK_OF_ART'), ("Dante Alighieri's", 'PERSON'), ('Purgatorio', 'PERSON'), ('Paradiso', 'PERSON'), ('Divine Comedy', 'PERSON'), ("William Blake's", 'PERSON'), ('Songs of Innocence', 'WORK_OF_ART'), ('Dante', 'PERSON'), ('Blake', 'ORG'), ('Feature', 'PRODUCT'), ('Dante', 'PERSON'), ('Divine Comedy', 'PERSON'), ('Blake', 'PERSON'), ('Songs of Innocence', 'WORK_OF_ART'), ('Dante', 'PERSON'), ('Christianity', 'NORP'), ('Language', 'LOC'), ('Christian', 'NORP'), ('Utilizes', 'ORG'), ('Blake', 'PERSON'), ('Dante', 'PERSON'), ('Divine Comedy', 'PERSON'), ('Virgil', 'PERSON'), ('the Garden of Eden', 'FAC'), ('Dante', 'PERSON'), ('Blake', 'PERSON'), ('Songs of Innocence', 'WORK_OF_ART'), ('Lamb', 'PERSON'), ('Tiger', 'PERSON'), ('Dante', 'PERSON'), ('Divine Comedy', 'PERSON'), ('Blake', 'PERSON'), ('Songs of Innocence', 'WORK_OF_ART')]</t>
+        </is>
+      </c>
       <c r="AE16" t="n">
         <v>68.69725823402405</v>
       </c>
@@ -3045,12 +3221,20 @@
       <c r="AZ16" t="inlineStr"/>
       <c r="BA16" t="inlineStr"/>
       <c r="BB16" t="inlineStr"/>
-      <c r="BC16" t="inlineStr"/>
-      <c r="BD16" t="inlineStr"/>
+      <c r="BC16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD16" t="n">
+        <v>3626</v>
+      </c>
       <c r="BE16" t="n">
         <v>24</v>
       </c>
-      <c r="BF16" t="inlineStr"/>
+      <c r="BF16" t="n">
+        <v>500</v>
+      </c>
       <c r="BG16" t="n">
         <v>784</v>
       </c>
@@ -3140,7 +3324,11 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>[('Japanese', 'NORP'), ('Impressionism', 'ORG'), ('Western', 'NORP'), ('Katsushika Hokusai', 'PERSON'), ('Utagawa Hiroshige', 'PERSON'), ('Impressionist', 'NORP'), ('Monet', 'PERSON'), ('Renoir', 'WORK_OF_ART'), ('Impressionist', 'NORP'), ('Capturing Daily Life:*', 'ORG'), ('Impressionism', 'ORG'), ('Cross-Cultural Exchange:*', 'ORG'), ('French', 'NORP'), ('Japanese', 'NORP'), ('Monet', 'PERSON'), ('"Water Lilies" Series', 'WORK_OF_ART'), ('Monet', 'PERSON'), ("Le Déjeuner sur l'herbe", 'WORK_OF_ART'), ('Impressionism', 'ORG'), ('Japanese', 'NORP'), ('Degas', 'PERSON'), ('Impressionism', 'ORG'), ('Impressionist', 'NORP')]</t>
+        </is>
+      </c>
       <c r="AE17" t="n">
         <v>57.68428087234497</v>
       </c>
@@ -3189,12 +3377,20 @@
       <c r="AZ17" t="inlineStr"/>
       <c r="BA17" t="inlineStr"/>
       <c r="BB17" t="inlineStr"/>
-      <c r="BC17" t="inlineStr"/>
-      <c r="BD17" t="inlineStr"/>
+      <c r="BC17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD17" t="n">
+        <v>3191</v>
+      </c>
       <c r="BE17" t="n">
         <v>19</v>
       </c>
-      <c r="BF17" t="inlineStr"/>
+      <c r="BF17" t="n">
+        <v>438</v>
+      </c>
       <c r="BG17" t="n">
         <v>653</v>
       </c>
@@ -3292,7 +3488,11 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="inlineStr"/>
-      <c r="AD18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>[('## Atonality', 'MONEY'), ('Arnold Schoenberg', 'PERSON'), ('20th-century', 'DATE'), ('Schoenberg', 'ORG'), ('Anton Webern', 'PERSON'), ('Alban Berg', 'PERSON'), ('the Intonation of the Sounds:*', 'ORG'), ('Complexity:*', 'ORG'), ('Ordering" Sounds:**', 'WORK_OF_ART'), ('20th-Century', 'DATE'), ('the Musical World:*', 'ORG'), ('Schoenberg', 'ORG'), ('20th-century', 'DATE'), ('Schoenberg', 'ORG'), ('Debussy &amp; Modernist Expression:*', 'ORG'), ('Schoenberg', 'ORG'), ('Debussy', 'PERSON'), ('Avant-Garde Compositions:*', 'ORG'), ('Dmitri Shostakovich', 'PERSON'), ('Pierre Boulez', 'PERSON'), ('Karlheinz Stockhausen', 'PERSON'), ('Schoenberg', 'ORG'), ('Schoenberg', 'ORG'), ('20th-century', 'DATE'), ('today', 'DATE'), ('serialist', 'NORP'), ('Schoenberg', 'ORG'), ('Arnold Schoenberg', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE18" t="n">
         <v>86.64069390296936</v>
       </c>
@@ -3341,12 +3541,20 @@
       <c r="AZ18" t="inlineStr"/>
       <c r="BA18" t="inlineStr"/>
       <c r="BB18" t="inlineStr"/>
-      <c r="BC18" t="inlineStr"/>
-      <c r="BD18" t="inlineStr"/>
+      <c r="BC18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD18" t="n">
+        <v>4486</v>
+      </c>
       <c r="BE18" t="n">
         <v>28</v>
       </c>
-      <c r="BF18" t="inlineStr"/>
+      <c r="BF18" t="n">
+        <v>626</v>
+      </c>
       <c r="BG18" t="n">
         <v>902</v>
       </c>
@@ -3444,7 +3652,11 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
-      <c r="AD19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>[('NLP', 'ORG'), ('1', 'CARDINAL'), ('RNN', 'ORG'), ('one', 'CARDINAL'), ('2', 'CARDINAL'), ('3', 'CARDINAL'), ('GPT', 'ORG'), ('Generative Pre-trained', 'PERSON'), ('Transformer', 'ORG'), ('BERT', 'ORG'), ('4', 'CARDINAL'), ('NLP Beyond Translation:*', 'ORG'), ('Question Answering:*', 'ORG'), ('NLP', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE19" t="n">
         <v>45.96540498733521</v>
       </c>
@@ -3493,12 +3705,20 @@
       <c r="AZ19" t="inlineStr"/>
       <c r="BA19" t="inlineStr"/>
       <c r="BB19" t="inlineStr"/>
-      <c r="BC19" t="inlineStr"/>
-      <c r="BD19" t="inlineStr"/>
+      <c r="BC19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD19" t="n">
+        <v>3340</v>
+      </c>
       <c r="BE19" t="n">
         <v>26</v>
       </c>
-      <c r="BF19" t="inlineStr"/>
+      <c r="BF19" t="n">
+        <v>418</v>
+      </c>
       <c r="BG19" t="n">
         <v>633</v>
       </c>
@@ -3594,7 +3814,11 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="inlineStr"/>
-      <c r="AD20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>[('## Fine', 'MONEY'), ('one', 'CARDINAL'), ('1', 'CARDINAL'), ('Pre-Trained Model:*', 'PERSON'), ('GPT-3', 'ORG'), ('BERT', 'ORG'), ('2', 'CARDINAL'), ('Adapt', 'FAC'), ('3', 'CARDINAL'), ('Transfer Learning:*', 'FAC'), ('Faster Training Time:*', 'PERSON'), ('BERT', 'ORG'), ('Question Answering:*', 'ORG'), ('GPT-3', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE20" t="n">
         <v>55.45954608917236</v>
       </c>
@@ -3643,12 +3867,20 @@
       <c r="AZ20" t="inlineStr"/>
       <c r="BA20" t="inlineStr"/>
       <c r="BB20" t="inlineStr"/>
-      <c r="BC20" t="inlineStr"/>
-      <c r="BD20" t="inlineStr"/>
+      <c r="BC20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD20" t="n">
+        <v>3528</v>
+      </c>
       <c r="BE20" t="n">
         <v>28</v>
       </c>
-      <c r="BF20" t="inlineStr"/>
+      <c r="BF20" t="n">
+        <v>484</v>
+      </c>
       <c r="BG20" t="n">
         <v>750</v>
       </c>
@@ -3750,7 +3982,11 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>[('##  Challenges', 'MONEY'), ('NLP', 'ORG'), ('1', 'CARDINAL'), ('Linguistic Nuances:*', 'ORG'), ('Sarcasm', 'ORG'), ('one', 'CARDINAL'), ('today', 'DATE'), ('summer day', 'DATE'), ('Irony', 'ORG'), ('Sarcasm', 'ORG'), ('2', 'CARDINAL'), ('Complexity of Emotional Expressions:*', 'ORG'), ('Sarcasm', 'ORG'), ('3', 'CARDINAL'), ('Data Limitations &amp; Model Bias:*', 'ORG'), ('Limited Training', 'ORG'), ('Sarcasm', 'ORG'), ('4.', 'CARDINAL'), ('Evolving Communication Styles:*', 'ORG'), ('BERT', 'ORG'), ('XLNet', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE21" t="n">
         <v>69.66839718818665</v>
       </c>
@@ -3799,12 +4035,20 @@
       <c r="AZ21" t="inlineStr"/>
       <c r="BA21" t="inlineStr"/>
       <c r="BB21" t="inlineStr"/>
-      <c r="BC21" t="inlineStr"/>
-      <c r="BD21" t="inlineStr"/>
+      <c r="BC21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD21" t="n">
+        <v>4547</v>
+      </c>
       <c r="BE21" t="n">
         <v>35</v>
       </c>
-      <c r="BF21" t="inlineStr"/>
+      <c r="BF21" t="n">
+        <v>633</v>
+      </c>
       <c r="BG21" t="n">
         <v>912</v>
       </c>
@@ -3910,7 +4154,11 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>[('## Advancements', 'MONEY'), ('1', 'CARDINAL'), ('NLU', 'ORG'), ('AI', 'ORG'), ('2', 'CARDINAL'), ('Dialogue Management &amp; Contextualization:*', 'ORG'), ('AI', 'ORG'), ('3', 'CARDINAL'), ('the Future of Human-AI Interaction:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('1', 'CARDINAL'), ('Personalization &amp; Empathy:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('2', 'CARDINAL'), ('Augmentation &amp; Productivity:*', 'ORG'), ('AI', 'ORG'), ('3', 'CARDINAL'), ('the Human-Machine Gap:*', 'ORG'), ('Challenges &amp; Ethical Considerations:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('Bias', 'PERSON'), ('AI', 'ORG'), ('AI:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE22" t="n">
         <v>57.94323682785034</v>
       </c>
@@ -3959,12 +4207,20 @@
       <c r="AZ22" t="inlineStr"/>
       <c r="BA22" t="inlineStr"/>
       <c r="BB22" t="inlineStr"/>
-      <c r="BC22" t="inlineStr"/>
-      <c r="BD22" t="inlineStr"/>
+      <c r="BC22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD22" t="n">
+        <v>3978</v>
+      </c>
       <c r="BE22" t="n">
         <v>26</v>
       </c>
-      <c r="BF22" t="inlineStr"/>
+      <c r="BF22" t="n">
+        <v>494</v>
+      </c>
       <c r="BG22" t="n">
         <v>771</v>
       </c>
@@ -4066,7 +4322,11 @@
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>[('AI Systems', 'ORG'), ('1', 'CARDINAL'), ('Data Representation &amp; Bias Mitigation:*', 'ORG'), ('Bias Detection &amp; Correction:*', 'ORG'), ('AI', 'ORG'), ('2', 'CARDINAL'), ('Content &amp; Language Understanding:*', 'ORG'), ('Cultural Sensitivity Training:*', 'ORG'), ('3', 'CARDINAL'), ('Ethical Considerations &amp; User Transparency:*', 'ORG'), ('User Consent &amp; Privacy:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('4', 'CARDINAL'), ('Continuous Learning &amp; Improvement:*', 'ORG'), ('Feedback Mechanisms:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('5', 'CARDINAL'), ('Responsible Deployment &amp; Community Engagement:*', 'ORG'), ('Cultural Sensitivity Guidelines:*', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('Challenges &amp; Limitations:*', 'ORG'), ('AI', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE23" t="n">
         <v>57.00896525382996</v>
       </c>
@@ -4115,12 +4375,20 @@
       <c r="AZ23" t="inlineStr"/>
       <c r="BA23" t="inlineStr"/>
       <c r="BB23" t="inlineStr"/>
-      <c r="BC23" t="inlineStr"/>
-      <c r="BD23" t="inlineStr"/>
+      <c r="BC23" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD23" t="n">
+        <v>4065</v>
+      </c>
       <c r="BE23" t="n">
         <v>31</v>
       </c>
-      <c r="BF23" t="inlineStr"/>
+      <c r="BF23" t="n">
+        <v>513</v>
+      </c>
       <c r="BG23" t="n">
         <v>768</v>
       </c>
@@ -4217,7 +4485,11 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>[('##', 'MONEY'), ('NLP', 'ORG'), ('1', 'CARDINAL'), ('one', 'CARDINAL'), ('English', 'LANGUAGE'), ('2', 'CARDINAL'), ('Limited Linguistic Resources:*', 'ORG'), ('NLP', 'ORG'), ('Idiom Variations', 'ORG'), ('Idioms', 'ORG'), ('3', 'CARDINAL'), ('Ambiguous Interpretations &amp; Potential for Miscommunication:*', 'ORG'), ('Humor &amp; Irony:*', 'ORG'), ('4', 'CARDINAL'), ('Bridging Linguistic &amp; Cultural Gaps:*', 'ORG'), ('5', 'CARDINAL'), ('Overcoming Challenges', 'ORG'), ('NLP', 'ORG'), ('Deep Learning &amp; Neural Networks:*', 'ORG'), ('Context-Aware Embeddings:*', 'ORG'), ('NLP', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE24" t="n">
         <v>53.43923115730286</v>
       </c>
@@ -4266,12 +4538,20 @@
       <c r="AZ24" t="inlineStr"/>
       <c r="BA24" t="inlineStr"/>
       <c r="BB24" t="inlineStr"/>
-      <c r="BC24" t="inlineStr"/>
-      <c r="BD24" t="inlineStr"/>
+      <c r="BC24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD24" t="n">
+        <v>3601</v>
+      </c>
       <c r="BE24" t="n">
         <v>29</v>
       </c>
-      <c r="BF24" t="inlineStr"/>
+      <c r="BF24" t="n">
+        <v>469</v>
+      </c>
       <c r="BG24" t="n">
         <v>732</v>
       </c>
@@ -4372,7 +4652,11 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
-      <c r="AD25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>[('## The Importance of Cultural Competence', 'MONEY'), ('AI Language Models', 'WORK_OF_ART'), ('AI language', 'FAC'), ('1', 'CARDINAL'), ('Bias', 'PERSON'), ('AI', 'ORG'), ('AI', 'ORG'), ('2', 'CARDINAL'), ('Promoting Accurate', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('3', 'CARDINAL'), ('AI', 'ORG'), ('4', 'CARDINAL'), ('Fostering Ethical AI Development:*', 'ORG'), ('AI', 'ORG'), ('AI language', 'FAC'), ('AI', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE25" t="n">
         <v>55.86469006538391</v>
       </c>
@@ -4421,12 +4705,20 @@
       <c r="AZ25" t="inlineStr"/>
       <c r="BA25" t="inlineStr"/>
       <c r="BB25" t="inlineStr"/>
-      <c r="BC25" t="inlineStr"/>
-      <c r="BD25" t="inlineStr"/>
+      <c r="BC25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD25" t="n">
+        <v>3878</v>
+      </c>
       <c r="BE25" t="n">
         <v>24</v>
       </c>
-      <c r="BF25" t="inlineStr"/>
+      <c r="BF25" t="n">
+        <v>491</v>
+      </c>
       <c r="BG25" t="n">
         <v>742</v>
       </c>
@@ -4538,7 +4830,11 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>[('##  Algorithm', 'MONEY'), ('1', 'CARDINAL'), ('CPU', 'ORG'), ('2', 'CARDINAL'), ('1', 'CARDINAL'), ('3', 'CARDINAL'), ('CPU', 'ORG'), ('two', 'CARDINAL'), ('1.5', 'CARDINAL'), ('2', 'CARDINAL'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('first', 'ORDINAL'), ('1', 'CARDINAL'), ('First', 'ORDINAL'), ('FCFS', 'ORG'), ('SJF', 'ORG'), ('2', 'CARDINAL'), ('Monitoring &amp; Adjustment:*', 'ORG'), ('1', 'CARDINAL'), ('Monitoring Execution Times', 'ORG'), ('2', 'CARDINAL'), ('3', 'CARDINAL'), ('Eigen', 'ORG'), ('4', 'CARDINAL'), ('Parallelism &amp; Multithreading:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE26" t="n">
         <v>76.56311798095703</v>
       </c>
@@ -4587,12 +4883,20 @@
       <c r="AZ26" t="inlineStr"/>
       <c r="BA26" t="inlineStr"/>
       <c r="BB26" t="inlineStr"/>
-      <c r="BC26" t="inlineStr"/>
-      <c r="BD26" t="inlineStr"/>
+      <c r="BC26" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD26" t="n">
+        <v>4264</v>
+      </c>
       <c r="BE26" t="n">
         <v>38</v>
       </c>
-      <c r="BF26" t="inlineStr"/>
+      <c r="BF26" t="n">
+        <v>526</v>
+      </c>
       <c r="BG26" t="n">
         <v>896</v>
       </c>
@@ -4701,7 +5005,11 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="inlineStr"/>
-      <c r="AD27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>[('## Trade', 'MONEY'), ('Privacy &amp; Security', 'ORG'), ('Digital Contact Tracing Systems', 'ORG'), ('Digital', 'ORG'), ('third', 'ORDINAL'), ('Data Minimization:*', 'ORG'), ('Access &amp; Correction:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE27" t="n">
         <v>64.36975145339966</v>
       </c>
@@ -4750,12 +5058,20 @@
       <c r="AZ27" t="inlineStr"/>
       <c r="BA27" t="inlineStr"/>
       <c r="BB27" t="inlineStr"/>
-      <c r="BC27" t="inlineStr"/>
-      <c r="BD27" t="inlineStr"/>
+      <c r="BC27" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD27" t="n">
+        <v>4170</v>
+      </c>
       <c r="BE27" t="n">
         <v>26</v>
       </c>
-      <c r="BF27" t="inlineStr"/>
+      <c r="BF27" t="n">
+        <v>516</v>
+      </c>
       <c r="BG27" t="n">
         <v>773</v>
       </c>
@@ -4859,7 +5175,11 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
-      <c r="AD28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>[('## Mitigating', 'MONEY'), ('I. Prevention &amp; Detection:*', 'ORG'), ('AI', 'ORG'), ('Response &amp; Accountability:*', 'ORG'), ('Collaboration &amp; Trust:*', 'ORG'), ('Ethical Considerations:*', 'ORG'), ('AI:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE28" t="n">
         <v>72.80426716804504</v>
       </c>
@@ -4908,12 +5228,20 @@
       <c r="AZ28" t="inlineStr"/>
       <c r="BA28" t="inlineStr"/>
       <c r="BB28" t="inlineStr"/>
-      <c r="BC28" t="inlineStr"/>
-      <c r="BD28" t="inlineStr"/>
+      <c r="BC28" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD28" t="n">
+        <v>4163</v>
+      </c>
       <c r="BE28" t="n">
         <v>24</v>
       </c>
-      <c r="BF28" t="inlineStr"/>
+      <c r="BF28" t="n">
+        <v>506</v>
+      </c>
       <c r="BG28" t="n">
         <v>837</v>
       </c>
@@ -5024,7 +5352,11 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="inlineStr"/>
-      <c r="AD29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>[('## A Sustainable Urban Transportation System', 'MONEY'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('Key Components:*', 'ORG'), ('Subway Network:*', 'ORG'), ('metro', 'ORG'), ('BRT', 'ORG'), ('Protected Bike Lanes &amp; Shared Paths:** Extensive', 'ORG'), ('Micro-Transit Service Network:*', 'ORG'), ('last-mile', 'QUANTITY'), ('Smart Technology Integration', 'ORG'), ('3', 'CARDINAL'), ('4', 'CARDINAL'), ('Universal Access Design:*', 'ORG'), ('5', 'CARDINAL'), ('Continuous Improvement &amp; Evaluation:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE29" t="n">
         <v>80.75700879096985</v>
       </c>
@@ -5073,12 +5405,20 @@
       <c r="AZ29" t="inlineStr"/>
       <c r="BA29" t="inlineStr"/>
       <c r="BB29" t="inlineStr"/>
-      <c r="BC29" t="inlineStr"/>
-      <c r="BD29" t="inlineStr"/>
+      <c r="BC29" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD29" t="n">
+        <v>4850</v>
+      </c>
       <c r="BE29" t="n">
         <v>30</v>
       </c>
-      <c r="BF29" t="inlineStr"/>
+      <c r="BF29" t="n">
+        <v>582</v>
+      </c>
       <c r="BG29" t="n">
         <v>915</v>
       </c>
@@ -5203,7 +5543,11 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="inlineStr"/>
-      <c r="AD30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>[('1', 'CARDINAL'), ('Data Collection &amp; Preparation:*', 'ORG'), ('Genomics Companies:*', 'ORG'), ('Data Cleaning &amp; Preprocessing:*', 'ORG'), ('-1', 'ORG'), ('1', 'CARDINAL'), ('one', 'CARDINAL'), ('SMOTE', 'PERSON'), ('2', 'CARDINAL'), ('Feature Engineering &amp; Selection:*', 'ORG'), ('Nucleotide Polymorphisms', 'PERSON'), ('Polygenic Risk Score', 'ORG'), ('Lifestyle Data:*', 'ORG'), ('Stress Levels:*', 'ORG'), ('PCA', 'ORG'), ('linear', 'ORG'), ('3', 'CARDINAL'), ('Model Selection &amp; Training:*', 'ORG'), ('Linear Regression', 'ORG'), ('Vector Machines', 'PERSON'), ('Decision Trees', 'PERSON'), ('Random Forests', 'PERSON'), ('Support Vector Classification', 'ORG'), ('Naive Bayes', 'PERSON'), ('K-Nearest Neighbors', 'ORG'), ('XGBoost', 'ORG'), ('LightGBM', 'ORG'), ('4', 'CARDINAL'), ('Model Evaluation &amp; Analysis:*', 'ORG'), ('F1', 'CARDINAL'), ('AUC', 'ORG'), ('5', 'CARDINAL'), ('6', 'CARDINAL'), ('Implementation &amp; Deployment:*', 'ORG'), ('Data Quality is Critical:*', 'ORG'), ('Collaboration &amp; Expertise:*', 'ORG'), ('clinicians', 'NORP'), ('Continuous Improvement:*', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE30" t="n">
         <v>92.6415958404541</v>
       </c>
@@ -5252,12 +5596,20 @@
       <c r="AZ30" t="inlineStr"/>
       <c r="BA30" t="inlineStr"/>
       <c r="BB30" t="inlineStr"/>
-      <c r="BC30" t="inlineStr"/>
-      <c r="BD30" t="inlineStr"/>
+      <c r="BC30" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD30" t="n">
+        <v>5093</v>
+      </c>
       <c r="BE30" t="n">
         <v>42</v>
       </c>
-      <c r="BF30" t="inlineStr"/>
+      <c r="BF30" t="n">
+        <v>605</v>
+      </c>
       <c r="BG30" t="n">
         <v>1147</v>
       </c>
@@ -5357,7 +5709,11 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="inlineStr"/>
-      <c r="AD31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>[('quantum entanglement', 'ORG'), ('Quantum Entanglement', 'ORG'), ('two', 'CARDINAL'), ('Alice', 'PERSON'), ('Bob', 'PERSON'), ('Alice', 'PERSON'), ('Bob', 'PERSON'), ('first', 'ORDINAL'), ('Shared State:*', 'ORG'), ('one', 'CARDINAL'), ('1', 'CARDINAL'), ('Quantum Cryptography:*', 'ORG'), ('two', 'CARDINAL'), ('third', 'ORDINAL'), ('2', 'CARDINAL'), ('Quantum Computing:*', 'ORG'), ('Quantum Algorithms:*', 'PERSON'), ('quantum entanglement', 'ORG'), ('Quantum Technologies:*', 'ORG'), ('quantum', 'ORG'), ('Applications Beyond Cryptography:*', 'PERSON'), ('GPS systems', 'ORG'), ('Nutshell', 'PERSON'), ('Quantum', 'ORG'), ('quantum', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE31" t="n">
         <v>52.81560754776001</v>
       </c>
@@ -5406,12 +5762,20 @@
       <c r="AZ31" t="inlineStr"/>
       <c r="BA31" t="inlineStr"/>
       <c r="BB31" t="inlineStr"/>
-      <c r="BC31" t="inlineStr"/>
-      <c r="BD31" t="inlineStr"/>
+      <c r="BC31" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD31" t="n">
+        <v>3167</v>
+      </c>
       <c r="BE31" t="n">
         <v>24</v>
       </c>
-      <c r="BF31" t="inlineStr"/>
+      <c r="BF31" t="n">
+        <v>418</v>
+      </c>
       <c r="BG31" t="n">
         <v>664</v>
       </c>
@@ -5512,7 +5876,11 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr"/>
       <c r="AC32" t="inlineStr"/>
-      <c r="AD32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>[('CRISPR-Cas9 Gene Editing', 'PERSON'), ('two', 'CARDINAL'), ('1', 'CARDINAL'), ('The Cas9 Enzyme:*', 'ORG'), ('2', 'CARDINAL'), ('Guide RNA', 'ORG'), ('RNA', 'ORG'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('Cas9', 'NORP'), ('3', 'CARDINAL'), ('Target Recognition &amp; Cut:*', 'ORG'), ('Cas9', 'NORP'), ('4', 'CARDINAL'), ('Two', 'CARDINAL'), ('HDR', 'ORG'), ('Cas9', 'NORP'), ('5', 'CARDINAL'), ('## Ethical Implications', 'MONEY'), ('CRISPR-Cas9', 'ORG'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('3', 'CARDINAL'), ('Social Inequality:*', 'ORG'), ('4.', 'CARDINAL'), ('CRISPR-Cas9', 'ORG'), ('5', 'CARDINAL'), ('Societal Acceptance:*', 'ORG'), ("CRISPR-Cas9's", 'ORG'), ('CRISPR-Cas9', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE32" t="n">
         <v>69.87185478210449</v>
       </c>
@@ -5561,12 +5929,20 @@
       <c r="AZ32" t="inlineStr"/>
       <c r="BA32" t="inlineStr"/>
       <c r="BB32" t="inlineStr"/>
-      <c r="BC32" t="inlineStr"/>
-      <c r="BD32" t="inlineStr"/>
+      <c r="BC32" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD32" t="n">
+        <v>3971</v>
+      </c>
       <c r="BE32" t="n">
         <v>36</v>
       </c>
-      <c r="BF32" t="inlineStr"/>
+      <c r="BF32" t="n">
+        <v>550</v>
+      </c>
       <c r="BG32" t="n">
         <v>830</v>
       </c>
@@ -5658,7 +6034,11 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
-      <c r="AD33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>[('two', 'CARDINAL'), ('about 95%', 'PERCENT'), ('Dark Matter:*', 'PERSON'), ('Microwave Background', 'PERSON'), ('CMB', 'ORG'), ('CMB', 'ORG'), ('the Big Bang', 'GPE'), ('Dark Energy:*', 'ORG'), ('about 68%', 'PERCENT'), ('Challenges and Ongoing Research:*', 'ORG'), ('Developing Models:**  Developing', 'WORK_OF_ART'), ('years', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE33" t="n">
         <v>55.60174441337585</v>
       </c>
@@ -5707,12 +6087,20 @@
       <c r="AZ33" t="inlineStr"/>
       <c r="BA33" t="inlineStr"/>
       <c r="BB33" t="inlineStr"/>
-      <c r="BC33" t="inlineStr"/>
-      <c r="BD33" t="inlineStr"/>
+      <c r="BC33" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD33" t="n">
+        <v>3399</v>
+      </c>
       <c r="BE33" t="n">
         <v>27</v>
       </c>
-      <c r="BF33" t="inlineStr"/>
+      <c r="BF33" t="n">
+        <v>494</v>
+      </c>
       <c r="BG33" t="n">
         <v>663</v>
       </c>
@@ -5807,7 +6195,11 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr"/>
       <c r="AC34" t="inlineStr"/>
-      <c r="AD34" t="inlineStr"/>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>[('## Challenges and', 'MONEY'), ('Developing Artificial General Intelligence', 'ORG'), ('Artificial General Intelligence', 'ORG'), ('AI', 'ORG'), ('AI', 'ORG'), ('AGI', 'ORG'), ('Data Requirements:*', 'ORG'), ('AGI', 'ORG'), ('AI', 'ORG'), ('AGI', 'ORG'), ('AGI', 'ORG'), ('Personalized Learning &amp; Healthcare', 'ORG'), ('AGI', 'ORG'), ('AGI', 'ORG'), ('AGI', 'ORG'), ('Focus on Ethical Development:*', 'ORG'), ('AI', 'ORG'), ('AGI', 'ORG'), ('AGI', 'ORG'), ('AGI', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE34" t="n">
         <v>62.8207323551178</v>
       </c>
@@ -5856,12 +6248,20 @@
       <c r="AZ34" t="inlineStr"/>
       <c r="BA34" t="inlineStr"/>
       <c r="BB34" t="inlineStr"/>
-      <c r="BC34" t="inlineStr"/>
-      <c r="BD34" t="inlineStr"/>
+      <c r="BC34" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD34" t="n">
+        <v>4243</v>
+      </c>
       <c r="BE34" t="n">
         <v>25</v>
       </c>
-      <c r="BF34" t="inlineStr"/>
+      <c r="BF34" t="n">
+        <v>543</v>
+      </c>
       <c r="BG34" t="n">
         <v>805</v>
       </c>
@@ -5958,7 +6358,11 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr"/>
       <c r="AC35" t="inlineStr"/>
-      <c r="AD35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>[('## Neuroplasticity', 'MONEY'), ('decades', 'DATE'), ('1', 'CARDINAL'), ('Learning &amp; Memory:*', 'ORG'), ('2', 'CARDINAL'), ('3', 'CARDINAL'), ('Brain Injury Recovery:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE35" t="n">
         <v>57.48736119270325</v>
       </c>
@@ -6007,12 +6411,20 @@
       <c r="AZ35" t="inlineStr"/>
       <c r="BA35" t="inlineStr"/>
       <c r="BB35" t="inlineStr"/>
-      <c r="BC35" t="inlineStr"/>
-      <c r="BD35" t="inlineStr"/>
+      <c r="BC35" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD35" t="n">
+        <v>3382</v>
+      </c>
       <c r="BE35" t="n">
         <v>28</v>
       </c>
-      <c r="BF35" t="inlineStr"/>
+      <c r="BF35" t="n">
+        <v>472</v>
+      </c>
       <c r="BG35" t="n">
         <v>698</v>
       </c>
@@ -6109,7 +6521,11 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr"/>
       <c r="AC36" t="inlineStr"/>
-      <c r="AD36" t="inlineStr"/>
+      <c r="AD36" t="inlineStr">
+        <is>
+          <t>[('7000', 'DATE'), ('64', 'CARDINAL'), ('128', 'CARDINAL'), ('192', 'CARDINAL'), ('GB', 'GPE'), ('3200', 'CARDINAL'), ('8', 'CARDINAL'), ('Redundant Power Supply and Fan Modules', 'WORK_OF_ART'), ('2x 10GbE', 'MONEY'), ('4x 2.5GbE Network Interfaces', 'QUANTITY'), ('5.0', 'CARDINAL'), ('Ethernet', 'PERSON'), ('Optional 10GbE Optical', 'ORG'), ('AI', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE36" t="n">
         <v>156.4974000453949</v>
       </c>
@@ -6158,12 +6574,20 @@
       <c r="AZ36" t="inlineStr"/>
       <c r="BA36" t="inlineStr"/>
       <c r="BB36" t="inlineStr"/>
-      <c r="BC36" t="inlineStr"/>
-      <c r="BD36" t="inlineStr"/>
+      <c r="BC36" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD36" t="n">
+        <v>1272</v>
+      </c>
       <c r="BE36" t="n">
         <v>8</v>
       </c>
-      <c r="BF36" t="inlineStr"/>
+      <c r="BF36" t="n">
+        <v>162</v>
+      </c>
       <c r="BG36" t="n">
         <v>292</v>
       </c>
@@ -6251,7 +6675,11 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr"/>
       <c r="AC37" t="inlineStr"/>
-      <c r="AD37" t="inlineStr"/>
+      <c r="AD37" t="inlineStr">
+        <is>
+          <t>[('Indian-American', 'NORP'), ('AngelList', 'ORG'), ('Investor &amp; Founder:*', 'ORG'), ('Uber, Airbnb', 'ORG'), ('Stripe', 'PRODUCT'), ('Reddit', 'NORP'), ('Author &amp; Speaker:**', 'ORG'), ('Mastering Bitcoin', 'WORK_OF_ART'), ('Reply All', 'WORK_OF_ART'), ('Key Aspects', 'ORG'), ('The Importance of Bitcoin:**', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE37" t="n">
         <v>43.1514458656311</v>
       </c>
@@ -6300,12 +6728,20 @@
       <c r="AZ37" t="inlineStr"/>
       <c r="BA37" t="inlineStr"/>
       <c r="BB37" t="inlineStr"/>
-      <c r="BC37" t="inlineStr"/>
-      <c r="BD37" t="inlineStr"/>
+      <c r="BC37" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD37" t="n">
+        <v>1791</v>
+      </c>
       <c r="BE37" t="n">
         <v>12</v>
       </c>
-      <c r="BF37" t="inlineStr"/>
+      <c r="BF37" t="n">
+        <v>249</v>
+      </c>
       <c r="BG37" t="n">
         <v>389</v>
       </c>
@@ -6409,7 +6845,11 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr"/>
       <c r="AC38" t="inlineStr"/>
-      <c r="AD38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr">
+        <is>
+          <t>[('## Chapter 1', 'MONEY'), ('The Echo Chamber', 'ORG'), ('Elena', 'ORG'), ('Earth', 'LOC'), ('Collective', 'PERSON'), ('Elena', 'ORG'), ('one', 'CARDINAL'), ('Exodus', 'PRODUCT'), ('Earth', 'LOC'), ('Earth', 'LOC'), ('Three', 'CARDINAL'), ('Pioneers', 'NORP'), ('Innovators', 'NORP'), ('Guardians', 'NORP'), ('Elena', 'ORG'), ('years', 'DATE'), ('one', 'CARDINAL'), ('The Pioneers', 'WORK_OF_ART'), ('Earth', 'LOC'), ('Guardians', 'NORP'), ('two feet', 'QUANTITY'), ('Pioneers', 'NORP'), ('Innovators', 'NORP'), ('Guardians', 'NORP'), ('Elena', 'ORG'), ('Elena', 'ORG'), ('first', 'ORDINAL'), ('Elena', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE38" t="n">
         <v>78.35348081588745</v>
       </c>
@@ -6458,12 +6898,20 @@
       <c r="AZ38" t="inlineStr"/>
       <c r="BA38" t="inlineStr"/>
       <c r="BB38" t="inlineStr"/>
-      <c r="BC38" t="inlineStr"/>
-      <c r="BD38" t="inlineStr"/>
+      <c r="BC38" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD38" t="n">
+        <v>4050</v>
+      </c>
       <c r="BE38" t="n">
         <v>27</v>
       </c>
-      <c r="BF38" t="inlineStr"/>
+      <c r="BF38" t="n">
+        <v>659</v>
+      </c>
       <c r="BG38" t="n">
         <v>793</v>
       </c>
@@ -6559,7 +7007,11 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr"/>
       <c r="AC39" t="inlineStr"/>
-      <c r="AD39" t="inlineStr"/>
+      <c r="AD39" t="inlineStr">
+        <is>
+          <t>[('##', 'MONEY'), ('P - Positive Changes:*', 'ORG'), ('1', 'CARDINAL'), ('2', 'CARDINAL'), ('SPIRE', 'ORG'), ('today', 'DATE'), ('daily', 'DATE'), ('3', 'CARDINAL'), ('4', 'CARDINAL'), ('SPIRE', 'ORG'), ('SPIRE', 'ORG'), ('daily', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE39" t="n">
         <v>51.07530093193054</v>
       </c>
@@ -6608,12 +7060,20 @@
       <c r="AZ39" t="inlineStr"/>
       <c r="BA39" t="inlineStr"/>
       <c r="BB39" t="inlineStr"/>
-      <c r="BC39" t="inlineStr"/>
-      <c r="BD39" t="inlineStr"/>
+      <c r="BC39" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD39" t="n">
+        <v>3121</v>
+      </c>
       <c r="BE39" t="n">
         <v>35</v>
       </c>
-      <c r="BF39" t="inlineStr"/>
+      <c r="BF39" t="n">
+        <v>464</v>
+      </c>
       <c r="BG39" t="n">
         <v>702</v>
       </c>
@@ -6709,7 +7169,11 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr"/>
       <c r="AC40" t="inlineStr"/>
-      <c r="AD40" t="inlineStr"/>
+      <c r="AD40" t="inlineStr">
+        <is>
+          <t>[('Wing Chun', 'PERSON'), ('Chinese', 'NORP'), ('Foshan', 'GPE'), ('Guangdong province', 'GPE'), ('China', 'GPE'), ('the 18th century', 'DATE'), ('Yim Wing Chun', 'PERSON'), ('Chinese', 'NORP'), ('Internal Energy Cultivation', 'ORG'), ('Chinese', 'NORP'), ('Hollywood', 'GPE'), ('Popularized Wing Chun', 'PERSON'), ('West', 'LOC'), ("Bruce Lee's", 'PERSON'), ('Jeet Kune', 'EVENT'), ('The Grandmaster', 'WORK_OF_ART'), ('millions', 'CARDINAL'), ('Wing Chun', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE40" t="n">
         <v>35.12794494628906</v>
       </c>
@@ -6758,12 +7222,20 @@
       <c r="AZ40" t="inlineStr"/>
       <c r="BA40" t="inlineStr"/>
       <c r="BB40" t="inlineStr"/>
-      <c r="BC40" t="inlineStr"/>
-      <c r="BD40" t="inlineStr"/>
+      <c r="BC40" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD40" t="n">
+        <v>2244</v>
+      </c>
       <c r="BE40" t="n">
         <v>15</v>
       </c>
-      <c r="BF40" t="inlineStr"/>
+      <c r="BF40" t="n">
+        <v>296</v>
+      </c>
       <c r="BG40" t="n">
         <v>481</v>
       </c>
@@ -6858,7 +7330,11 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr"/>
       <c r="AC41" t="inlineStr"/>
-      <c r="AD41" t="inlineStr"/>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>[('Morihei Ueshiba', 'PERSON'), ('1904-1969', 'DATE'), ('Japanese', 'NORP'), ('Aikido', 'GPE'), ('Aikido', 'PERSON'), ('today', 'DATE'), ('Aikido', 'PERSON'), ('the early 20th century', 'DATE'), ('Japanese', 'NORP'), ('Ueshiba', 'ORG'), ('Aikido', 'NORP'), ('Aikido', 'PERSON'), ('Ueshiba', 'ORG'), ('Oshogaki', 'WORK_OF_ART'), ('Ueshiba', 'ORG'), ('Aikido', 'GPE'), ('Ueshiba', 'ORG'), ('Martial Arts:*', 'ORG'), ('Aikido', 'PERSON'), ('Health &amp; Self-Improvement:*', 'ORG'), ('Ueshiba', 'ORG'), ('Morihei Ueshiba', 'PERSON'), ('Aikido', 'PERSON'), ('the Aikikai Hombu Dojo', 'ORG'), ('Tokyo', 'GPE'), ('Articles', 'PERSON'), ('Ueshiba', 'ORG'), ('The Art of Aikido', 'WORK_OF_ART'), ('Ueshiba', 'ORG'), ('Aikido: The Way of Peace', 'WORK_OF_ART'), ("Morihei Ueshiba's", 'PERSON'), ('Aikido', 'GPE')]</t>
+        </is>
+      </c>
       <c r="AE41" t="n">
         <v>41.54534721374512</v>
       </c>
@@ -6907,12 +7383,20 @@
       <c r="AZ41" t="inlineStr"/>
       <c r="BA41" t="inlineStr"/>
       <c r="BB41" t="inlineStr"/>
-      <c r="BC41" t="inlineStr"/>
-      <c r="BD41" t="inlineStr"/>
+      <c r="BC41" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD41" t="n">
+        <v>2554</v>
+      </c>
       <c r="BE41" t="n">
         <v>17</v>
       </c>
-      <c r="BF41" t="inlineStr"/>
+      <c r="BF41" t="n">
+        <v>346</v>
+      </c>
       <c r="BG41" t="n">
         <v>585</v>
       </c>
@@ -7001,7 +7485,11 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr"/>
       <c r="AC42" t="inlineStr"/>
-      <c r="AD42" t="inlineStr"/>
+      <c r="AD42" t="inlineStr">
+        <is>
+          <t>[('Miyamoto Musashi', 'PERSON'), ('1584-1645', 'DATE'), ('Japanese', 'NORP'), ('one', 'CARDINAL'), ('Musashi', 'PERSON'), ('Two', 'CARDINAL'), ('two', 'CARDINAL'), ('The Way of the Sword', 'WORK_OF_ART'), ('The Art of Disappearances', 'WORK_OF_ART'), ('Legendary Battles:*', 'PERSON'), ('Musashi', 'PERSON'), ('Sasaki Kojiro', 'GPE'), ('Musashi', 'PERSON'), ('Literary Legacy', 'PERSON'), ('The Book of Five Rings:*', 'WORK_OF_ART'), ('Musashi', 'PERSON'), ('the centuries', 'DATE'), ('Miyamoto Musashi', 'PERSON'), ('Japanese', 'NORP'), ('today', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE42" t="n">
         <v>30.71544909477234</v>
       </c>
@@ -7050,12 +7538,20 @@
       <c r="AZ42" t="inlineStr"/>
       <c r="BA42" t="inlineStr"/>
       <c r="BB42" t="inlineStr"/>
-      <c r="BC42" t="inlineStr"/>
-      <c r="BD42" t="inlineStr"/>
+      <c r="BC42" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD42" t="n">
+        <v>1773</v>
+      </c>
       <c r="BE42" t="n">
         <v>13</v>
       </c>
-      <c r="BF42" t="inlineStr"/>
+      <c r="BF42" t="n">
+        <v>264</v>
+      </c>
       <c r="BG42" t="n">
         <v>409</v>
       </c>
@@ -7148,7 +7644,11 @@
       <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
-      <c r="AD43" t="inlineStr"/>
+      <c r="AD43" t="inlineStr">
+        <is>
+          <t>[('The Book of Five Rings', 'WORK_OF_ART'), ('Miyamoto Musashi', 'PERSON'), ('Japanese', 'NORP'), ('the 17th century', 'DATE'), ('five', 'CARDINAL'), ('Samurai', 'PERSON'), ('Musashi', 'PERSON'), ('first', 'ORDINAL'), ('The Book of Five Rings', 'WORK_OF_ART'), ('between 1645-1649', 'DATE'), ('Musashi', 'PERSON'), ('Edo', 'ORG'), ('The "Book of Five Rings', 'WORK_OF_ART'), ('The Book of Five Rings', 'WORK_OF_ART')]</t>
+        </is>
+      </c>
       <c r="AE43" t="n">
         <v>43.87992238998413</v>
       </c>
@@ -7197,12 +7697,20 @@
       <c r="AZ43" t="inlineStr"/>
       <c r="BA43" t="inlineStr"/>
       <c r="BB43" t="inlineStr"/>
-      <c r="BC43" t="inlineStr"/>
-      <c r="BD43" t="inlineStr"/>
+      <c r="BC43" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD43" t="n">
+        <v>2619</v>
+      </c>
       <c r="BE43" t="n">
         <v>21</v>
       </c>
-      <c r="BF43" t="inlineStr"/>
+      <c r="BF43" t="n">
+        <v>386</v>
+      </c>
       <c r="BG43" t="n">
         <v>536</v>
       </c>
@@ -7300,7 +7808,11 @@
       <c r="AA44" t="inlineStr"/>
       <c r="AB44" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
-      <c r="AD44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>[('Society &amp; Culture:*', 'ORG'), ('Redefined Art &amp; Creativity:*', 'ORG'), ('New Social Structures:*', 'ORG'), ('Challenges &amp; Potential Solutions:*', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE44" t="n">
         <v>44.28774833679199</v>
       </c>
@@ -7349,12 +7861,20 @@
       <c r="AZ44" t="inlineStr"/>
       <c r="BA44" t="inlineStr"/>
       <c r="BB44" t="inlineStr"/>
-      <c r="BC44" t="inlineStr"/>
-      <c r="BD44" t="inlineStr"/>
+      <c r="BC44" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD44" t="n">
+        <v>2666</v>
+      </c>
       <c r="BE44" t="n">
         <v>20</v>
       </c>
-      <c r="BF44" t="inlineStr"/>
+      <c r="BF44" t="n">
+        <v>365</v>
+      </c>
       <c r="BG44" t="n">
         <v>529</v>
       </c>
@@ -7450,7 +7970,11 @@
       <c r="AA45" t="inlineStr"/>
       <c r="AB45" t="inlineStr"/>
       <c r="AC45" t="inlineStr"/>
-      <c r="AD45" t="inlineStr"/>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t>[('ActivityPub', 'ORG'), ('Twitter', 'PERSON'), ('Fediverse', 'PERSON'), ('Fediverse', 'PERSON'), ('Reddit', 'NORP'), ('Discord', 'GPE'), ('Mastodon', 'GPE'), ('Mastodon', 'PERSON'), ('Twitter', 'PERSON'), ('YouTube', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE45" t="n">
         <v>41.97327995300293</v>
       </c>
@@ -7499,12 +8023,20 @@
       <c r="AZ45" t="inlineStr"/>
       <c r="BA45" t="inlineStr"/>
       <c r="BB45" t="inlineStr"/>
-      <c r="BC45" t="inlineStr"/>
-      <c r="BD45" t="inlineStr"/>
+      <c r="BC45" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD45" t="n">
+        <v>2424</v>
+      </c>
       <c r="BE45" t="n">
         <v>19</v>
       </c>
-      <c r="BF45" t="inlineStr"/>
+      <c r="BF45" t="n">
+        <v>330</v>
+      </c>
       <c r="BG45" t="n">
         <v>524</v>
       </c>
@@ -7597,7 +8129,11 @@
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>[('Walden', 'WORK_OF_ART'), ('Henry David Thoreau', 'PERSON'), ('1', 'CARDINAL'), ('Simplicity &amp; Self-Reliance:*', 'ORG'), ('Thoreau', 'ORG'), ('Walden Pond', 'FAC'), ('two years', 'DATE'), ('2', 'CARDINAL'), ('3', 'CARDINAL'), ('Walden', 'WORK_OF_ART'), ('Freedom &amp; Conformity:*', 'ORG'), ('4', 'CARDINAL'), ('Reflection on Society &amp; Technology:*', 'ORG'), ('Thoreau', 'ORG'), ('Walden', 'GPE'), ('today', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE46" t="n">
         <v>47.14622807502747</v>
       </c>
@@ -7646,12 +8182,20 @@
       <c r="AZ46" t="inlineStr"/>
       <c r="BA46" t="inlineStr"/>
       <c r="BB46" t="inlineStr"/>
-      <c r="BC46" t="inlineStr"/>
-      <c r="BD46" t="inlineStr"/>
+      <c r="BC46" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD46" t="n">
+        <v>2687</v>
+      </c>
       <c r="BE46" t="n">
         <v>23</v>
       </c>
-      <c r="BF46" t="inlineStr"/>
+      <c r="BF46" t="n">
+        <v>396</v>
+      </c>
       <c r="BG46" t="n">
         <v>556</v>
       </c>
@@ -7767,7 +8311,11 @@
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
-      <c r="AD47" t="inlineStr"/>
+      <c r="AD47" t="inlineStr">
+        <is>
+          <t>[('weekly', 'DATE'), ('Week 1 - Focus', 'DATE'), ('Legs &amp; Core', 'ORG'), ('5 minutes', 'TIME'), ('3', 'CARDINAL'), ('8-12', 'CARDINAL'), ('3', 'CARDINAL'), ('8-12', 'CARDINAL'), ('3', 'CARDINAL'), ('15-20', 'CARDINAL'), ('30 seconds', 'TIME'), ('3', 'CARDINAL'), ('3', 'CARDINAL'), ('15-20', 'CARDINAL'), ('5 minutes', 'TIME'), ('30 seconds', 'TIME'), ('Week 2 - Focus', 'DATE'), ('5 minutes', 'TIME'), ('3', 'CARDINAL'), ('3', 'CARDINAL'), ('8-12', 'CARDINAL'), ('3', 'CARDINAL'), ('8-12', 'CARDINAL'), ('45 seconds', 'TIME'), ('3', 'CARDINAL'), ('3', 'CARDINAL'), ('10-12', 'CARDINAL'), ('5 minutes', 'TIME'), ('Week 3 - Focus', 'DATE'), ('5 minutes', 'TIME'), ('3', 'CARDINAL'), ('8-10', 'CARDINAL'), ('3', 'CARDINAL'), ('8-12', 'CARDINAL'), ('Romanian Deadlifts', 'PERSON'), ('3', 'CARDINAL'), ('8-12', 'CARDINAL'), ('3', 'CARDINAL'), ('3', 'CARDINAL'), ('15-20', 'CARDINAL'), ('5 minutes', 'TIME'), ('Week 4 - Focus', 'DATE'), ('5 minutes', 'TIME'), ('30-45 minutes', 'TIME'), ('Include', 'ORG'), ('Russian', 'NORP'), ('5 minutes', 'TIME'), ('each week', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE47" t="n">
         <v>81.08618760108948</v>
       </c>
@@ -7816,12 +8364,20 @@
       <c r="AZ47" t="inlineStr"/>
       <c r="BA47" t="inlineStr"/>
       <c r="BB47" t="inlineStr"/>
-      <c r="BC47" t="inlineStr"/>
-      <c r="BD47" t="inlineStr"/>
+      <c r="BC47" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD47" t="n">
+        <v>3456</v>
+      </c>
       <c r="BE47" t="n">
         <v>22</v>
       </c>
-      <c r="BF47" t="inlineStr"/>
+      <c r="BF47" t="n">
+        <v>512</v>
+      </c>
       <c r="BG47" t="n">
         <v>859</v>
       </c>
@@ -7921,7 +8477,11 @@
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
-      <c r="AD48" t="inlineStr"/>
+      <c r="AD48" t="inlineStr">
+        <is>
+          <t>[('1', 'CARDINAL'), ('third', 'ORDINAL'), ('2', 'CARDINAL'), ('Model Focus:*', 'PERSON'), ('Gmail', 'PERSON'), ('Amazon', 'ORG'), ('3', 'CARDINAL'), ('Complex Data Structures:*', 'ORG'), ('jargon', 'ORG'), ('Data:*', 'ORG'), ('4', 'CARDINAL'), ('Competition &amp; Market Dynamics:*', 'ORG'), ('Competitive Advantage:*', 'ORG'), ('5', 'CARDINAL'), ('Balancing Privacy &amp; Innovation:*', 'ORG'), ('Paramount', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE48" t="n">
         <v>61.49904298782349</v>
       </c>
@@ -7970,12 +8530,20 @@
       <c r="AZ48" t="inlineStr"/>
       <c r="BA48" t="inlineStr"/>
       <c r="BB48" t="inlineStr"/>
-      <c r="BC48" t="inlineStr"/>
-      <c r="BD48" t="inlineStr"/>
+      <c r="BC48" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD48" t="n">
+        <v>3883</v>
+      </c>
       <c r="BE48" t="n">
         <v>33</v>
       </c>
-      <c r="BF48" t="inlineStr"/>
+      <c r="BF48" t="n">
+        <v>551</v>
+      </c>
       <c r="BG48" t="n">
         <v>763</v>
       </c>
@@ -8061,7 +8629,11 @@
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
       <c r="AC49" t="inlineStr"/>
-      <c r="AD49" t="inlineStr"/>
+      <c r="AD49" t="inlineStr">
+        <is>
+          <t>[('## Fight Club', 'MONEY'), ('Chapter 1 - A New Type of Echo', 'LAW'), ('Tyler', 'PERSON'), ('Tyler', 'PERSON'), ('a thousand', 'CARDINAL'), ('Tyler', 'PERSON'), ('night', 'TIME'), ('Tyler', 'PERSON'), ('Tyler', 'ORG'), ('Tyler', 'ORG')]</t>
+        </is>
+      </c>
       <c r="AE49" t="n">
         <v>54.21773481369019</v>
       </c>
@@ -8110,12 +8682,20 @@
       <c r="AZ49" t="inlineStr"/>
       <c r="BA49" t="inlineStr"/>
       <c r="BB49" t="inlineStr"/>
-      <c r="BC49" t="inlineStr"/>
-      <c r="BD49" t="inlineStr"/>
+      <c r="BC49" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD49" t="n">
+        <v>2876</v>
+      </c>
       <c r="BE49" t="n">
         <v>30</v>
       </c>
-      <c r="BF49" t="inlineStr"/>
+      <c r="BF49" t="n">
+        <v>525</v>
+      </c>
       <c r="BG49" t="n">
         <v>643</v>
       </c>
@@ -8198,7 +8778,11 @@
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>[('a clear day', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE50" t="n">
         <v>20.15048408508301</v>
       </c>
@@ -8247,12 +8831,20 @@
       <c r="AZ50" t="inlineStr"/>
       <c r="BA50" t="inlineStr"/>
       <c r="BB50" t="inlineStr"/>
-      <c r="BC50" t="inlineStr"/>
-      <c r="BD50" t="inlineStr"/>
+      <c r="BC50" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD50" t="n">
+        <v>506</v>
+      </c>
       <c r="BE50" t="n">
         <v>7</v>
       </c>
-      <c r="BF50" t="inlineStr"/>
+      <c r="BF50" t="n">
+        <v>81</v>
+      </c>
       <c r="BG50" t="n">
         <v>108</v>
       </c>
@@ -8328,7 +8920,11 @@
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>[('Christmas', 'DATE'), ('December 25th', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE51" t="n">
         <v>23.97223591804504</v>
       </c>
@@ -8377,12 +8973,20 @@
       <c r="AZ51" t="inlineStr"/>
       <c r="BA51" t="inlineStr"/>
       <c r="BB51" t="inlineStr"/>
-      <c r="BC51" t="inlineStr"/>
-      <c r="BD51" t="inlineStr"/>
+      <c r="BC51" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD51" t="n">
+        <v>154</v>
+      </c>
       <c r="BE51" t="n">
         <v>2</v>
       </c>
-      <c r="BF51" t="inlineStr"/>
+      <c r="BF51" t="n">
+        <v>27</v>
+      </c>
       <c r="BG51" t="n">
         <v>34</v>
       </c>
@@ -8458,7 +9062,11 @@
       <c r="AA52" t="inlineStr"/>
       <c r="AB52" t="inlineStr"/>
       <c r="AC52" t="inlineStr"/>
-      <c r="AD52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="AE52" t="n">
         <v>12.93182849884033</v>
       </c>
@@ -8508,11 +9116,15 @@
       <c r="BA52" t="inlineStr"/>
       <c r="BB52" t="inlineStr"/>
       <c r="BC52" t="inlineStr"/>
-      <c r="BD52" t="inlineStr"/>
+      <c r="BD52" t="n">
+        <v>71</v>
+      </c>
       <c r="BE52" t="n">
         <v>2</v>
       </c>
-      <c r="BF52" t="inlineStr"/>
+      <c r="BF52" t="n">
+        <v>16</v>
+      </c>
       <c r="BG52" t="n">
         <v>19</v>
       </c>
@@ -8588,7 +9200,11 @@
       <c r="AA53" t="inlineStr"/>
       <c r="AB53" t="inlineStr"/>
       <c r="AC53" t="inlineStr"/>
-      <c r="AD53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>[('Mount Everest', 'LOC'), ('8,848.86 meters', 'QUANTITY'), ('29,032.6 feet', 'QUANTITY')]</t>
+        </is>
+      </c>
       <c r="AE53" t="n">
         <v>13.47611379623413</v>
       </c>
@@ -8637,12 +9253,20 @@
       <c r="AZ53" t="inlineStr"/>
       <c r="BA53" t="inlineStr"/>
       <c r="BB53" t="inlineStr"/>
-      <c r="BC53" t="inlineStr"/>
-      <c r="BD53" t="inlineStr"/>
+      <c r="BC53" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD53" t="n">
+        <v>101</v>
+      </c>
       <c r="BE53" t="n">
         <v>1</v>
       </c>
-      <c r="BF53" t="inlineStr"/>
+      <c r="BF53" t="n">
+        <v>17</v>
+      </c>
       <c r="BG53" t="n">
         <v>31</v>
       </c>
@@ -8718,7 +9342,11 @@
       <c r="AA54" t="inlineStr"/>
       <c r="AB54" t="inlineStr"/>
       <c r="AC54" t="inlineStr"/>
-      <c r="AD54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t>[('100 degrees Celsius', 'QUANTITY'), ('212 degrees', 'QUANTITY'), ('Fahrenheit', 'WORK_OF_ART')]</t>
+        </is>
+      </c>
       <c r="AE54" t="n">
         <v>10.59204339981079</v>
       </c>
@@ -8767,12 +9395,20 @@
       <c r="AZ54" t="inlineStr"/>
       <c r="BA54" t="inlineStr"/>
       <c r="BB54" t="inlineStr"/>
-      <c r="BC54" t="inlineStr"/>
-      <c r="BD54" t="inlineStr"/>
+      <c r="BC54" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD54" t="n">
+        <v>197</v>
+      </c>
       <c r="BE54" t="n">
         <v>3</v>
       </c>
-      <c r="BF54" t="inlineStr"/>
+      <c r="BF54" t="n">
+        <v>34</v>
+      </c>
       <c r="BG54" t="n">
         <v>44</v>
       </c>
@@ -8849,7 +9485,11 @@
       <c r="AA55" t="inlineStr"/>
       <c r="AB55" t="inlineStr"/>
       <c r="AC55" t="inlineStr"/>
-      <c r="AD55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>[('7 days', 'DATE'), ('a week', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE55" t="n">
         <v>11.29056572914124</v>
       </c>
@@ -8899,11 +9539,15 @@
       <c r="BA55" t="inlineStr"/>
       <c r="BB55" t="inlineStr"/>
       <c r="BC55" t="inlineStr"/>
-      <c r="BD55" t="inlineStr"/>
+      <c r="BD55" t="n">
+        <v>119</v>
+      </c>
       <c r="BE55" t="n">
         <v>2</v>
       </c>
-      <c r="BF55" t="inlineStr"/>
+      <c r="BF55" t="n">
+        <v>23</v>
+      </c>
       <c r="BG55" t="n">
         <v>28</v>
       </c>
@@ -8979,7 +9623,11 @@
       <c r="AA56" t="inlineStr"/>
       <c r="AB56" t="inlineStr"/>
       <c r="AC56" t="inlineStr"/>
-      <c r="AD56" t="inlineStr"/>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>[('Harper Lee', 'PERSON'), ('1926', 'DATE'), ('New Orleans', 'GPE'), ('Louisiana', 'GPE'), ('American', 'NORP'), ('Lee', 'PERSON'), ('Mockingbird', 'GPE'), ('Lee', 'PERSON')]</t>
+        </is>
+      </c>
       <c r="AE56" t="n">
         <v>16.28455948829651</v>
       </c>
@@ -9028,12 +9676,20 @@
       <c r="AZ56" t="inlineStr"/>
       <c r="BA56" t="inlineStr"/>
       <c r="BB56" t="inlineStr"/>
-      <c r="BC56" t="inlineStr"/>
-      <c r="BD56" t="inlineStr"/>
+      <c r="BC56" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD56" t="n">
+        <v>390</v>
+      </c>
       <c r="BE56" t="n">
         <v>4</v>
       </c>
-      <c r="BF56" t="inlineStr"/>
+      <c r="BF56" t="n">
+        <v>69</v>
+      </c>
       <c r="BG56" t="n">
         <v>82</v>
       </c>
@@ -9110,7 +9766,11 @@
       <c r="AA57" t="inlineStr"/>
       <c r="AB57" t="inlineStr"/>
       <c r="AC57" t="inlineStr"/>
-      <c r="AD57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>[('1', 'CARDINAL'), ('3', 'CARDINAL')]</t>
+        </is>
+      </c>
       <c r="AE57" t="n">
         <v>4.63580060005188</v>
       </c>
@@ -9159,12 +9819,20 @@
       <c r="AZ57" t="inlineStr"/>
       <c r="BA57" t="inlineStr"/>
       <c r="BB57" t="inlineStr"/>
-      <c r="BC57" t="inlineStr"/>
-      <c r="BD57" t="inlineStr"/>
+      <c r="BC57" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD57" t="n">
+        <v>53</v>
+      </c>
       <c r="BE57" t="n">
         <v>2</v>
       </c>
-      <c r="BF57" t="inlineStr"/>
+      <c r="BF57" t="n">
+        <v>11</v>
+      </c>
       <c r="BG57" t="n">
         <v>17</v>
       </c>
@@ -9240,7 +9908,11 @@
       <c r="AA58" t="inlineStr"/>
       <c r="AB58" t="inlineStr"/>
       <c r="AC58" t="inlineStr"/>
-      <c r="AD58" t="inlineStr"/>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>[('Christmas', 'DATE'), ('Christians', 'NORP'), ('December 25th to January 1st', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE58" t="n">
         <v>14.12414336204529</v>
       </c>
@@ -9289,12 +9961,20 @@
       <c r="AZ58" t="inlineStr"/>
       <c r="BA58" t="inlineStr"/>
       <c r="BB58" t="inlineStr"/>
-      <c r="BC58" t="inlineStr"/>
-      <c r="BD58" t="inlineStr"/>
+      <c r="BC58" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD58" t="n">
+        <v>115</v>
+      </c>
       <c r="BE58" t="n">
         <v>2</v>
       </c>
-      <c r="BF58" t="inlineStr"/>
+      <c r="BF58" t="n">
+        <v>19</v>
+      </c>
       <c r="BG58" t="n">
         <v>21</v>
       </c>
@@ -9370,7 +10050,11 @@
       <c r="AA59" t="inlineStr"/>
       <c r="AB59" t="inlineStr"/>
       <c r="AC59" t="inlineStr"/>
-      <c r="AD59" t="inlineStr"/>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="AE59" t="n">
         <v>5.235190391540527</v>
       </c>
@@ -9419,12 +10103,20 @@
       <c r="AZ59" t="inlineStr"/>
       <c r="BA59" t="inlineStr"/>
       <c r="BB59" t="inlineStr"/>
-      <c r="BC59" t="inlineStr"/>
-      <c r="BD59" t="inlineStr"/>
+      <c r="BC59" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BD59" t="n">
+        <v>85</v>
+      </c>
       <c r="BE59" t="n">
         <v>2</v>
       </c>
-      <c r="BF59" t="inlineStr"/>
+      <c r="BF59" t="n">
+        <v>18</v>
+      </c>
       <c r="BG59" t="n">
         <v>21</v>
       </c>
@@ -9501,7 +10193,11 @@
       <c r="AA60" t="inlineStr"/>
       <c r="AB60" t="inlineStr"/>
       <c r="AC60" t="inlineStr"/>
-      <c r="AD60" t="inlineStr"/>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>[('France', 'GPE'), ('Paris', 'GPE')]</t>
+        </is>
+      </c>
       <c r="AE60" t="n">
         <v>3.900015830993652</v>
       </c>
@@ -9551,11 +10247,15 @@
       <c r="BA60" t="inlineStr"/>
       <c r="BB60" t="inlineStr"/>
       <c r="BC60" t="inlineStr"/>
-      <c r="BD60" t="inlineStr"/>
+      <c r="BD60" t="n">
+        <v>33</v>
+      </c>
       <c r="BE60" t="n">
         <v>1</v>
       </c>
-      <c r="BF60" t="inlineStr"/>
+      <c r="BF60" t="n">
+        <v>6</v>
+      </c>
       <c r="BG60" t="n">
         <v>7</v>
       </c>
@@ -9631,7 +10331,11 @@
       <c r="AA61" t="inlineStr"/>
       <c r="AB61" t="inlineStr"/>
       <c r="AC61" t="inlineStr"/>
-      <c r="AD61" t="inlineStr"/>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>[('7 days', 'DATE'), ('a week', 'DATE'), ('every 7 days', 'DATE')]</t>
+        </is>
+      </c>
       <c r="AE61" t="n">
         <v>4.950026988983154</v>
       </c>
@@ -9681,11 +10385,15 @@
       <c r="BA61" t="inlineStr"/>
       <c r="BB61" t="inlineStr"/>
       <c r="BC61" t="inlineStr"/>
-      <c r="BD61" t="inlineStr"/>
+      <c r="BD61" t="n">
+        <v>79</v>
+      </c>
       <c r="BE61" t="n">
         <v>2</v>
       </c>
-      <c r="BF61" t="inlineStr"/>
+      <c r="BF61" t="n">
+        <v>17</v>
+      </c>
       <c r="BG61" t="n">
         <v>19</v>
       </c>
@@ -9761,7 +10469,11 @@
       <c r="AA62" t="inlineStr"/>
       <c r="AB62" t="inlineStr"/>
       <c r="AC62" t="inlineStr"/>
-      <c r="AD62" t="inlineStr"/>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t>[('Jupiter', 'LOC'), ('318', 'CARDINAL'), ('Earth', 'LOC'), ('143,892 kilometers', 'QUANTITY'), ('1.431 billion cubic kilometers', 'QUANTITY')]</t>
+        </is>
+      </c>
       <c r="AE62" t="n">
         <v>8.451048374176025</v>
       </c>
@@ -9811,11 +10523,15 @@
       <c r="BA62" t="inlineStr"/>
       <c r="BB62" t="inlineStr"/>
       <c r="BC62" t="inlineStr"/>
-      <c r="BD62" t="inlineStr"/>
+      <c r="BD62" t="n">
+        <v>167</v>
+      </c>
       <c r="BE62" t="n">
         <v>2</v>
       </c>
-      <c r="BF62" t="inlineStr"/>
+      <c r="BF62" t="n">
+        <v>30</v>
+      </c>
       <c r="BG62" t="n">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
updating for 2x variance benchmarks
</commit_message>
<xml_diff>
--- a/prompt_responses_rated.xlsx
+++ b/prompt_responses_rated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BQ60"/>
+  <dimension ref="A1:CC60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,6 +777,66 @@
       <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>Img_Seed</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Accuracy_Rating</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Accuracy_Explain</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Clarity_Rating</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Clarity_Explain</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Relevance_Rating</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Relevance_Explain</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Adherence_Rating</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Adherence_Explain</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Insight_Rating</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Insight_Explain</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Variance_Rating</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>Mistral_Variance_Explain</t>
         </is>
       </c>
     </row>
@@ -1009,6 +1069,54 @@
       <c r="BO2" t="inlineStr"/>
       <c r="BP2" t="inlineStr"/>
       <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS2" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and largely accurate overview of the latest developments in quantum computing as of 2024 and their implications for cryptography, though the absence of specific, recent real-world examples slightly reduces its accuracy.</t>
+        </is>
+      </c>
+      <c r="BT2" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a clear overview of the latest developments in quantum computing and their implications for cryptography, although some sections contain technical jargon that might require prior knowledge for full understanding.</t>
+        </is>
+      </c>
+      <c r="BV2" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the latest developments in quantum computing as of 2024 and discusses their potential implications for cryptography, closely aligning with the prompt.</t>
+        </is>
+      </c>
+      <c r="BX2" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY2" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed explanation of the latest developments in quantum computing as of 2024 and discusses the potential implications for cryptography, closely following the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ2" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA2" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and nuanced overview of the latest developments in quantum computing and its implications for cryptography, showcasing a deep understanding of the subject matter.</t>
+        </is>
+      </c>
+      <c r="CB2" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC2" t="inlineStr">
+        <is>
+          <t>While both messages cover the latest developments in quantum computing and their implications for cryptography, Message A provides a more detailed and comprehensive overview, including specific advancements in hardware, software, and applications, which are not all mentioned in Message B. However, the core themes and implications for cryptography are consistent between the two messages.</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1219,6 +1327,54 @@
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="inlineStr"/>
       <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>The response correctly identifies that the report in question is from 2021 and accurately summarizes the key findings of the IPCC AR6 report, providing a detailed and factually correct summary.</t>
+        </is>
+      </c>
+      <c r="BT3" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>The response is well-structured and easy to understand, clearly outlining the key findings of the IPCC AR6 report from 2021, but it slightly deviates from the prompt's specific request for the 2024 report.</t>
+        </is>
+      </c>
+      <c r="BV3" t="n">
+        <v>5</v>
+      </c>
+      <c r="BW3" t="inlineStr">
+        <is>
+          <t>The response provides detailed information on the IPCC report from 2021, which is somewhat relevant but does not address the specific request for the 2024 report.</t>
+        </is>
+      </c>
+      <c r="BX3" t="n">
+        <v>5</v>
+      </c>
+      <c r="BY3" t="inlineStr">
+        <is>
+          <t>The response acknowledges the prompt's request for information on a future IPCC report but primarily discusses the 2021 report, thereby only partially adhering to the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ3" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA3" t="inlineStr">
+        <is>
+          <t>While the response effectively summarizes the key findings of the IPCC AR6 report from 2021, it misses the opportunity to delve deeper into the implications or provide forward-looking insights that might be expected in a 2024 report.</t>
+        </is>
+      </c>
+      <c r="CB3" t="n">
+        <v>7</v>
+      </c>
+      <c r="CC3" t="inlineStr">
+        <is>
+          <t>Message A discusses the IPCC report from 2021, focusing on findings that were already established, while Message B specifically addresses the 2024 report, highlighting new developments such as global temperatures exceeding 1.5°C and the need for stronger international cooperation, which are not covered in Message A.</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1439,6 +1595,54 @@
       <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="inlineStr"/>
       <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS4" t="inlineStr">
+        <is>
+          <t>The response provides a generally accurate overview of the Artemis program, its current status, and future prospects, but contains a few minor inaccuracies and outdated information, such as the timeline for the Artemis II mission and the status of the Lunar Gateway.</t>
+        </is>
+      </c>
+      <c r="BT4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, effectively conveying the current status and future prospects of the Artemis program.</t>
+        </is>
+      </c>
+      <c r="BV4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW4" t="inlineStr">
+        <is>
+          <t>The response directly addresses the current status, future prospects, and goals of the Artemis program for lunar exploration, providing comprehensive and relevant information as required by the prompt.</t>
+        </is>
+      </c>
+      <c r="BX4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY4" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the current status and future prospects of the Artemis program, detailing its goals for lunar exploration as instructed in the prompt.</t>
+        </is>
+      </c>
+      <c r="BZ4" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA4" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and well-structured overview of the Artemis program, detailing its current status, future prospects, goals, and challenges, demonstrating a deep understanding and thoughtful consideration of the topic.</t>
+        </is>
+      </c>
+      <c r="CB4" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC4" t="inlineStr">
+        <is>
+          <t>While Message A provides more detailed and expanded information, it largely aligns with the key points of Message B, including the current status, future prospects, and goals of the Artemis program, with only minor differences in specific details and timelines.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1666,6 +1870,54 @@
       <c r="BO5" t="inlineStr"/>
       <c r="BP5" t="inlineStr"/>
       <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS5" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and mostly accurate overview of recent breakthroughs in CRISPR technology and their potential applications in medicine. It covers key advancements like base editing and prime editing, as well as applications in cancer therapy, genetic diseases, and infectious diseases. However, it slightly overstates the current impact of CRISPR on certain diseases and does not delve into the nuances of challenges and ethical concerns as deeply as it could, which keeps it from a perfect score.</t>
+        </is>
+      </c>
+      <c r="BT5" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU5" t="inlineStr">
+        <is>
+          <t>The response is highly clear and easy to understand, with a well-organized structure, detailed explanations, and specific examples illustrating recent breakthroughs and applications in CRISPR technology.</t>
+        </is>
+      </c>
+      <c r="BV5" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW5" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive overview of recent breakthroughs in CRISPR technology and their potential medical applications, directly addressing the prompt with highly relevant information.</t>
+        </is>
+      </c>
+      <c r="BX5" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY5" t="inlineStr">
+        <is>
+          <t>The response fully adheres to the prompt by providing a comprehensive overview of recent breakthroughs in CRISPR technology and their potential applications in medicine.</t>
+        </is>
+      </c>
+      <c r="BZ5" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA5" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed overview of CRISPR technology, highlighting recent advancements and potential applications in medicine, while also acknowledging challenges and ethical concerns.</t>
+        </is>
+      </c>
+      <c r="CB5" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC5" t="inlineStr">
+        <is>
+          <t>While Message A provides more detailed information and additional applications, the core concepts and potential medical applications of CRISPR technology, such as treating genetic disorders and cancer, are present in both messages, indicating a moderate level of variance.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1889,6 +2141,54 @@
       <c r="BO6" t="inlineStr"/>
       <c r="BP6" t="inlineStr"/>
       <c r="BQ6" t="inlineStr"/>
+      <c r="BR6" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>The response accurately acknowledges that the 2024 Nobel Prize in Physics has not yet been announced and provides a well-informed discussion of potential candidates and significant research areas, though it does not specify the actual award-winning research since it is not yet determined.</t>
+        </is>
+      </c>
+      <c r="BT6" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU6" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides detailed information about potential contenders for the 2024 Nobel Prize in Physics, but it becomes somewhat convoluted due to the extensive details and multiple subtopics, which could be streamlined for better clarity.</t>
+        </is>
+      </c>
+      <c r="BV6" t="n">
+        <v>3</v>
+      </c>
+      <c r="BW6" t="inlineStr">
+        <is>
+          <t>The response provides general information about potential candidates and research areas for the Nobel Prize in Physics but does not specifically address the significance of the 2024 Nobel Prize or describe the research that led to the award, as the prompt requested.</t>
+        </is>
+      </c>
+      <c r="BX6" t="n">
+        <v>3</v>
+      </c>
+      <c r="BY6" t="inlineStr">
+        <is>
+          <t>The response does not explain the significance of the 2024 Nobel Prize in Physics nor describe the specific research that led to the award, instead discussing potential contenders and research areas.</t>
+        </is>
+      </c>
+      <c r="BZ6" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA6" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and detailed overview of potential areas that could lead to the 2024 Nobel Prize in Physics, demonstrating knowledge and thoughtfulness, but it lacks specific predictions or deeper analysis of current research trends.</t>
+        </is>
+      </c>
+      <c r="CB6" t="n">
+        <v>8</v>
+      </c>
+      <c r="CC6" t="inlineStr">
+        <is>
+          <t>Message A speculates on potential candidates and research areas for the 2024 Nobel Prize in Physics, while Message B specifically identifies the awarded research and its significance, resulting in a high variance due to the lack of concrete details and differing focus in Message A.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2109,6 +2409,54 @@
       <c r="BO7" t="inlineStr"/>
       <c r="BP7" t="inlineStr"/>
       <c r="BQ7" t="inlineStr"/>
+      <c r="BR7" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS7" t="inlineStr">
+        <is>
+          <t>The response accurately discusses potential impacts of a hypothetical 2024 global energy crisis on renewable energy adoption and international relations, providing a comprehensive and well-reasoned analysis.</t>
+        </is>
+      </c>
+      <c r="BT7" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU7" t="inlineStr">
+        <is>
+          <t>The response is well-structured and articulate, clearly presenting the potential impacts of a global energy crisis on renewable energy adoption and international relations, although the use of some technical terms might slightly reduce its accessibility to a general audience.</t>
+        </is>
+      </c>
+      <c r="BV7" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW7" t="inlineStr">
+        <is>
+          <t>The response thoroughly addresses the impact of the 2024 global energy crisis on both renewable energy adoption and international relations, with detailed and relevant points for each aspect.</t>
+        </is>
+      </c>
+      <c r="BX7" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY7" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt, thoroughly discussing the impact of the 2024 global energy crisis on both renewable energy adoption and international relations, with detailed points and clear structure.</t>
+        </is>
+      </c>
+      <c r="BZ7" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA7" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and thoughtful analysis of the potential impacts of a 2024 global energy crisis on renewable energy adoption and international relations, highlighting key challenges and opportunities with nuanced consideration.</t>
+        </is>
+      </c>
+      <c r="CB7" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC7" t="inlineStr">
+        <is>
+          <t>While both messages discuss the impact of a 2024 global energy crisis on renewable energy adoption and international relations, Message A provides a more detailed and hypothetical analysis with specific points, whereas Message B presents a concise overview of actual events and impacts, leading to some variance in substance and detail, but not in the overall meaning.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2335,6 +2683,54 @@
       <c r="BO8" t="inlineStr"/>
       <c r="BP8" t="inlineStr"/>
       <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS8" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and well-balanced analysis of the 2024 economic outlook for emerging markets, accurately identifying key factors influencing growth, such as global recovery, structural reforms, inflationary pressures, and geopolitical uncertainties.</t>
+        </is>
+      </c>
+      <c r="BT8" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU8" t="inlineStr">
+        <is>
+          <t>The response is well-structured and presents a clear, detailed analysis of the 2024 economic outlook for emerging markets, with distinct sections addressing driving factors, challenges, regional analysis, and potential scenarios.</t>
+        </is>
+      </c>
+      <c r="BV8" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW8" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed analysis of the 2024 economic outlook for emerging markets, directly addressing the prompt's requirements by discussing factors influencing growth, challenges, regional analysis, and potential scenarios.</t>
+        </is>
+      </c>
+      <c r="BX8" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY8" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and comprehensive analysis of the 2024 economic outlook for emerging markets, addressing both growth factors and challenges, and offers regional insights as well as potential scenarios, closely aligning with the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ8" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA8" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive, balanced, and thoughtful analysis of the 2024 economic outlook for emerging markets, covering a wide range of factors and presenting well-reasoned scenarios.</t>
+        </is>
+      </c>
+      <c r="CB8" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC8" t="inlineStr">
+        <is>
+          <t>While both messages discuss the 2024 economic outlook for emerging markets, highlighting growth factors and challenges, Message A provides a more detailed and structured analysis, including regional breakdowns and scenarios, which Message B lacks, leading to a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2565,6 +2961,54 @@
       <c r="BO9" t="inlineStr"/>
       <c r="BP9" t="inlineStr"/>
       <c r="BQ9" t="inlineStr"/>
+      <c r="BR9" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS9" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and largely accurate overview of recent advancements in fusion energy research and its potential impact on the energy sector, though it omits specific details about ongoing challenges and the exact timeline of achievements.</t>
+        </is>
+      </c>
+      <c r="BT9" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU9" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a clear and detailed explanation of recent advancements in fusion energy research and their potential impact on the energy sector.</t>
+        </is>
+      </c>
+      <c r="BV9" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW9" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses recent advancements in fusion energy research and their potential to revolutionize the energy sector, aligning perfectly with the prompt.</t>
+        </is>
+      </c>
+      <c r="BX9" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY9" t="inlineStr">
+        <is>
+          <t>The response closely follows the prompt's instructions by explaining recent advancements in fusion energy research and their potential to revolutionize the energy sector, with detailed and relevant information.</t>
+        </is>
+      </c>
+      <c r="BZ9" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA9" t="inlineStr">
+        <is>
+          <t>The response provides a thorough, detailed, and well-structured overview of recent advancements in fusion energy research, effectively highlighting the potential and challenges, which demonstrates a deep understanding and thoughtful analysis of the topic.</t>
+        </is>
+      </c>
+      <c r="CB9" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC9" t="inlineStr">
+        <is>
+          <t>While both messages discuss recent advancements in fusion energy and their potential impact, Message A provides more detailed examples and additional aspects such as inertial confinement fusion and challenges, which are not covered in Message B, leading to a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2811,6 +3255,54 @@
       <c r="BO10" t="inlineStr"/>
       <c r="BP10" t="inlineStr"/>
       <c r="BQ10" t="inlineStr"/>
+      <c r="BR10" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS10" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and generally accurate overview of FeFETs, their features, advantages, applications, challenges, and future prospects, as well as the role of hafnia-based ferroelectrics and 2D materials. However, slight inaccuracies in specific details, such as the switching speeds of traditional transistors and FeFETs, reduce the accuracy score slightly.</t>
+        </is>
+      </c>
+      <c r="BT10" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU10" t="inlineStr">
+        <is>
+          <t>The response is well-organized and provides a comprehensive explanation of FeFETs, including key features, advantages, applications, and challenges, making it easy to understand despite the complex subject matter.</t>
+        </is>
+      </c>
+      <c r="BV10" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW10" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and comprehensive explanation of FeFETs, covering their key features, advantages, applications, challenges, and future prospects, as well as discussing hafnia-based ferroelectrics and 2D materials, all of which are directly relevant to the prompt.</t>
+        </is>
+      </c>
+      <c r="BX10" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY10" t="inlineStr">
+        <is>
+          <t>The response comprehensively covers the prompt's requirements, providing detailed explanations of FeFETs, their advantages, applications, and challenges, including the role of hafnia-based ferroelectrics and 2D materials.</t>
+        </is>
+      </c>
+      <c r="BZ10" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA10" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed explanation of FeFETs, highlighting their key features, advantages, applications, and challenges, and includes insightful discussion on the role of hafnia-based ferroelectrics and 2D materials.</t>
+        </is>
+      </c>
+      <c r="CB10" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC10" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and comprehensive explanation, it closely aligns with the key points and advantages of FeFETs mentioned in Message B, such as non-volatility, low power consumption, and faster switching speeds. The main difference lies in the level of detail, but the core substance and meaning remain consistent.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3042,6 +3534,54 @@
       <c r="BO11" t="inlineStr"/>
       <c r="BP11" t="inlineStr"/>
       <c r="BQ11" t="inlineStr"/>
+      <c r="BR11" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS11" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and balanced overview of the potential implications of a Universal Basic Income policy, accurately discussing both positive and negative aspects related to employment, poverty, economic growth, and social structures, while also considering various stakeholder perspectives.</t>
+        </is>
+      </c>
+      <c r="BT11" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU11" t="inlineStr">
+        <is>
+          <t>The response is well-structured, comprehensive, and easy to understand, clearly outlining the potential positive and negative implications of a Universal Basic Income policy in the United States.</t>
+        </is>
+      </c>
+      <c r="BV11" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW11" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt's request to discuss the potential implications of adopting a Universal Basic Income (UBI) policy in the United States, covering effects on employment, poverty, economic growth, and social structures, as well as perspectives from various stakeholders.</t>
+        </is>
+      </c>
+      <c r="BX11" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY11" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the prompt's requirements by discussing both positive and negative implications of UBI on employment, poverty, economic growth, and social structures, and includes perspectives from economists, politicians, and citizens.</t>
+        </is>
+      </c>
+      <c r="BZ11" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA11" t="inlineStr">
+        <is>
+          <t>The response provides a balanced and thoughtful discussion, covering a wide range of potential implications and stakeholder perspectives, and offers a nuanced conclusion that advocates for careful consideration and evidence-based decision-making.</t>
+        </is>
+      </c>
+      <c r="CB11" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC11" t="inlineStr">
+        <is>
+          <t>While both messages discuss the implications of UBI, Message A provides more detailed analysis and additional points, such as social mobility and moral hazard, leading to a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3280,6 +3820,54 @@
       <c r="BO12" t="inlineStr"/>
       <c r="BP12" t="inlineStr"/>
       <c r="BQ12" t="inlineStr"/>
+      <c r="BR12" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS12" t="inlineStr">
+        <is>
+          <t>The response accurately outlines the challenges, impacts, and benefits of a sudden switch to electric vehicles, providing a detailed and largely correct assessment of the implications for the power grid and electricity availability.</t>
+        </is>
+      </c>
+      <c r="BT12" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU12" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, though some sentences are complex and could be simplified for better clarity.</t>
+        </is>
+      </c>
+      <c r="BV12" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW12" t="inlineStr">
+        <is>
+          <t>The response addresses the prompt directly by discussing the impacts of an overnight switch to electric vehicles on the power grid and electricity availability, including detailed considerations of challenges, potential impacts, and realistic scenarios.</t>
+        </is>
+      </c>
+      <c r="BX12" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY12" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and relevant discussion on the implications of switching from gas vehicles to electric vehicles on the power grid and electricity availability, though it deviates slightly by discussing broader impacts and realistic scenarios.</t>
+        </is>
+      </c>
+      <c r="BZ12" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA12" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and balanced analysis of the hypothetical scenario, addressing both challenges and advantages, and offers realistic solutions, demonstrating a thoughtful and insightful approach.</t>
+        </is>
+      </c>
+      <c r="CB12" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC12" t="inlineStr">
+        <is>
+          <t>While both messages address the impact of an overnight switch to electric vehicles on the power grid and electricity availability, Message A provides a more detailed and structured breakdown, including potential advantages and challenges, whereas Message B focuses more concisely on the immediate implications and necessary adjustments. The core substance and meaning are largely similar, but the depth and breadth of discussion differ, warranting a moderate variance rating of 3.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3503,6 +4091,54 @@
       <c r="BO13" t="inlineStr"/>
       <c r="BP13" t="inlineStr"/>
       <c r="BQ13" t="inlineStr"/>
+      <c r="BR13" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS13" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and accurate analysis of the use of stream of consciousness in James Joyce's "Ulysses" and its impact on modernist literature, covering key aspects such as interiority, fluid time and space, and internal monologues, as well as the broader impact on literary conventions and psychology.</t>
+        </is>
+      </c>
+      <c r="BT13" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU13" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a clear, detailed analysis of the stream of consciousness technique in "Ulysses" and its impact on modernist literature, using specific examples and explanations.</t>
+        </is>
+      </c>
+      <c r="BV13" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW13" t="inlineStr">
+        <is>
+          <t>The response comprehensively analyzes the use of stream of consciousness in James Joyce's "Ulysses" and its substantial impact on modernist literature, closely aligning with the prompt.</t>
+        </is>
+      </c>
+      <c r="BX13" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY13" t="inlineStr">
+        <is>
+          <t>The response comprehensively analyzes the use of stream of consciousness in "Ulysses" and discusses its impact on modernist literature, closely adhering to the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ13" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA13" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and thoughtful analysis of the stream of consciousness technique in "Ulysses," thoroughly exploring its impact on modernist literature and beyond, with a strong understanding of the text and its context.</t>
+        </is>
+      </c>
+      <c r="CB13" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC13" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and expansive analysis of the stream of consciousness technique in "Ulysses" and its impact on modernist literature, including specific examples and broad context, it retains the core substance and meaning of Message B, hence a moderate variance rating.</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3722,6 +4358,54 @@
       <c r="BO14" t="inlineStr"/>
       <c r="BP14" t="inlineStr"/>
       <c r="BQ14" t="inlineStr"/>
+      <c r="BR14" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS14" t="inlineStr">
+        <is>
+          <t>The response accurately discusses the role of absurdism in "Waiting for Godot" and its reflection of post-World War II existential thought, with detailed and appropriate references to the play's themes and characters.</t>
+        </is>
+      </c>
+      <c r="BT14" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU14" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a clear analysis of absurdism in "Waiting for Godot" and its connection to post-World War II existential thought, though some sentences are complex and could be simplified for better understanding.</t>
+        </is>
+      </c>
+      <c r="BV14" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW14" t="inlineStr">
+        <is>
+          <t>The response thoroughly discusses the role of absurdism in "Waiting for Godot" and effectively ties it to post-World War II existential thought, with only minor details that could be considered tangential.</t>
+        </is>
+      </c>
+      <c r="BX14" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY14" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt by thoroughly discussing the role of absurdism in "Waiting for Godot" and effectively linking it to post-World War II existential thought.</t>
+        </is>
+      </c>
+      <c r="BZ14" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA14" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and nuanced exploration of the themes of absurdism and existentialism in "Waiting for Godot," effectively linking them to the post-World War II context and offering a balanced perspective on the play's message.</t>
+        </is>
+      </c>
+      <c r="CB14" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC14" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and expansive discussion, it largely aligns with the core themes and ideas presented in Message B, discussing the role of absurdism and post-World War II existential thought in "Waiting for Godot."</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3950,6 +4634,54 @@
       <c r="BO15" t="inlineStr"/>
       <c r="BP15" t="inlineStr"/>
       <c r="BQ15" t="inlineStr"/>
+      <c r="BR15" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS15" t="inlineStr">
+        <is>
+          <t>The response accurately compares and contrasts the use of symbolism and allegory in Dante's "Divine Comedy" and William Blake's "Songs of Innocence and of Experience," providing detailed and factually correct information about both works.</t>
+        </is>
+      </c>
+      <c r="BT15" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU15" t="inlineStr">
+        <is>
+          <t>The response is well-structured and effectively compares and contrasts the use of symbolism and allegory in both works, with clear and organized points, though minor improvements in conciseness could enhance clarity further.</t>
+        </is>
+      </c>
+      <c r="BV15" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW15" t="inlineStr">
+        <is>
+          <t>The response comprehensively and directly addresses the use of symbolism and allegory in both Dante's "Divine Comedy" and William Blake's "Songs of Innocence and of Experience," providing detailed comparisons and contrasts as required by the prompt.</t>
+        </is>
+      </c>
+      <c r="BX15" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY15" t="inlineStr">
+        <is>
+          <t>The response effectively compares and contrasts the use of symbolism and allegory in Dante's "Divine Comedy" and William Blake's "Songs of Innocence and of Experience," providing detailed analysis and examples aligned with the prompt.</t>
+        </is>
+      </c>
+      <c r="BZ15" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA15" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and balanced comparison, delving into the specifics of symbolism and allegory in both works and offering clear contrasts, which demonstrates a strong understanding and thoughtful analysis.</t>
+        </is>
+      </c>
+      <c r="CB15" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC15" t="inlineStr">
+        <is>
+          <t>While Message A and Message B both discuss the use of symbolism and allegory in Dante's "Divine Comedy" and William Blake's "Songs of Innocence and of Experience," Message A provides a more detailed and structured comparison, including a table and specific examples, which expands upon the benchmark's concise overview.</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4168,6 +4900,54 @@
       <c r="BO16" t="inlineStr"/>
       <c r="BP16" t="inlineStr"/>
       <c r="BQ16" t="inlineStr"/>
+      <c r="BR16" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS16" t="inlineStr">
+        <is>
+          <t>The response accurately describes the influence of Japanese ukiyo-e woodblock prints on Impressionism, highlighting key artists and specific techniques that were adopted, but it slightly exaggerates the direct influence on techniques like sfumato, which is more associated with the Renaissance.</t>
+        </is>
+      </c>
+      <c r="BT16" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU16" t="inlineStr">
+        <is>
+          <t>The response is exceptionally clear and well-structured, with distinct sections addressing direct and indirect influences, examples, and impact, making it easy to understand the connection between Japanese ukiyo-e woodblock prints and Impressionism.</t>
+        </is>
+      </c>
+      <c r="BV16" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW16" t="inlineStr">
+        <is>
+          <t>The response is entirely focused on examining the influence of Japanese ukiyo-e woodblock prints on the development of Impressionism in late 19th-century European art, providing detailed and relevant information that directly addresses the prompt.</t>
+        </is>
+      </c>
+      <c r="BX16" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY16" t="inlineStr">
+        <is>
+          <t>The response meticulously addresses the prompt by thoroughly examining the influence of Japanese ukiyo-e woodblock prints on the development of Impressionism, providing detailed examples and analysis.</t>
+        </is>
+      </c>
+      <c r="BZ16" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA16" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed analysis of the influence of Japanese ukiyo-e woodblock prints on Impressionism, highlighting both direct and indirect influences, and offering specific examples to support the discussion.</t>
+        </is>
+      </c>
+      <c r="CB16" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC16" t="inlineStr">
+        <is>
+          <t>While both messages highlight the influence of Japanese ukiyo-e woodblock prints on Impressionism, Message A provides significantly more detailed examples and analysis, including direct and indirect influences, which are not present in Message B. However, the core substance and meaning regarding the impact of ukiyo-e on Impressionism remain consistent between the two messages.</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -4398,6 +5178,54 @@
       <c r="BO17" t="inlineStr"/>
       <c r="BP17" t="inlineStr"/>
       <c r="BQ17" t="inlineStr"/>
+      <c r="BR17" t="n">
+        <v>7</v>
+      </c>
+      <c r="BS17" t="inlineStr">
+        <is>
+          <t>The response provides a generally accurate overview of Arnold Schoenberg's use of atonality and serialism, and their impact on 20th-century classical music, but it contains some minor inaccuracies and oversimplifications, such as the misattribution of impressionism to Schoenberg's influence and the overstatement of serialism's reliance on "scales."</t>
+        </is>
+      </c>
+      <c r="BT17" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU17" t="inlineStr">
+        <is>
+          <t>The response provides a clear and detailed analysis of atonality and serialism in Arnold Schoenberg's compositions and their impact on 20th-century classical music, with well-organized sections and straightforward language.</t>
+        </is>
+      </c>
+      <c r="BV17" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW17" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and focused analysis of Arnold Schoenberg's use of atonality and serialism and their impact on 20th-century classical music, aligning closely with the prompt.</t>
+        </is>
+      </c>
+      <c r="BX17" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY17" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt by analyzing atonality and serialism in Schoenberg's compositions and their impact on 20th-century classical music, though it includes some extraneous details about other composers and styles that slightly dilute the focus.</t>
+        </is>
+      </c>
+      <c r="BZ17" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA17" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive, detailed, and thoughtful analysis of Schoenberg's use of atonality and serialism, highlighting their significant impact on 20th-century classical music with well-explained examples and a nuanced understanding of the subject matter.</t>
+        </is>
+      </c>
+      <c r="CB17" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC17" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and expansive explanation of atonality and serialism in Schoenberg's work, it largely aligns with the core concepts presented in Message B, maintaining a similar substance and meaning with additional elaboration.</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -4621,6 +5449,54 @@
       <c r="BO18" t="inlineStr"/>
       <c r="BP18" t="inlineStr"/>
       <c r="BQ18" t="inlineStr"/>
+      <c r="BR18" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS18" t="inlineStr">
+        <is>
+          <t>The response accurately explains the concept of transformers in NLP and their impact on machine translation, covering key aspects like the attention mechanism and parallel processing, although minor inaccuracies and overstatements slightly reduce the score.</t>
+        </is>
+      </c>
+      <c r="BT18" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU18" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to follow, providing clear explanations of transformers and their impact on machine translation.</t>
+        </is>
+      </c>
+      <c r="BV18" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW18" t="inlineStr">
+        <is>
+          <t>The response provides a detailed explanation of transformers in NLP and their impact on machine translation, directly addressing the prompt, though some additional information on broader NLP applications slightly dilutes the focus.</t>
+        </is>
+      </c>
+      <c r="BX18" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY18" t="inlineStr">
+        <is>
+          <t>The response comprehensively explains the concept of transformers in NLP and their impact on machine translation, but it also includes additional information about other NLP applications that slightly deviates from the core focus of the prompt.</t>
+        </is>
+      </c>
+      <c r="BZ18" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA18" t="inlineStr">
+        <is>
+          <t>The response provides a clear and detailed explanation of transformers, their key features, and how they revolutionized machine translation, offering a thorough and insightful overview.</t>
+        </is>
+      </c>
+      <c r="CB18" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC18" t="inlineStr">
+        <is>
+          <t>Message A provides a more detailed and expansive explanation of transformers and their impact on NLP compared to Message B, but the core concepts and revolutionary aspects highlighted are substantially similar.</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -4849,6 +5725,54 @@
       <c r="BO19" t="inlineStr"/>
       <c r="BP19" t="inlineStr"/>
       <c r="BQ19" t="inlineStr"/>
+      <c r="BR19" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS19" t="inlineStr">
+        <is>
+          <t>The response accurately describes the process and benefits of transfer learning in fine-tuning language models, providing detailed and correct information about pre-trained models, task-specific fine-tuning, and domain adaptation.</t>
+        </is>
+      </c>
+      <c r="BT19" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU19" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a clear explanation of how transfer learning is applied in fine-tuning language models for specific tasks, including detailed steps and benefits.</t>
+        </is>
+      </c>
+      <c r="BV19" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW19" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by thoroughly explaining how transfer learning is applied in fine-tuning language models for specific tasks, including detailed steps, benefits, examples, and challenges.</t>
+        </is>
+      </c>
+      <c r="BX19" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY19" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses how transfer learning is applied in fine-tuning language models for specific tasks, with detailed explanations and examples, fully adhering to the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ19" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA19" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive, detailed, and well-structured explanation of transfer learning in fine-tuning language models, including its benefits, applications, and challenges.</t>
+        </is>
+      </c>
+      <c r="CB19" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC19" t="inlineStr">
+        <is>
+          <t>While Message A provides more detailed examples and additional context, the core substance and meaning of transfer learning in fine-tuning language models align closely with Message B.</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -5078,6 +6002,54 @@
       <c r="BO20" t="inlineStr"/>
       <c r="BP20" t="inlineStr"/>
       <c r="BQ20" t="inlineStr"/>
+      <c r="BR20" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS20" t="inlineStr">
+        <is>
+          <t>The response accurately identifies and explains the key challenges in detecting sarcasm and irony in sentiment analysis, covering linguistic nuances, complexity of emotional expressions, data limitations, and evolving communication styles.</t>
+        </is>
+      </c>
+      <c r="BT20" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU20" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, with clear examples that illustrate the challenges of detecting sarcasm and irony in sentiment analysis.</t>
+        </is>
+      </c>
+      <c r="BV20" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW20" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by analyzing various challenges in sentiment analysis for detecting sarcasm and irony, including linguistic nuances, emotional expressions, data limitations, and evolving communication styles.</t>
+        </is>
+      </c>
+      <c r="BX20" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY20" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt by thoroughly analyzing the challenges of sentiment analysis in detecting sarcasm and irony, providing detailed examples and addressing potential solutions.</t>
+        </is>
+      </c>
+      <c r="BZ20" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA20" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and nuanced exploration of the challenges in detecting sarcasm and irony in sentiment analysis, supported by clear examples and thoughtful suggestions for improvement.</t>
+        </is>
+      </c>
+      <c r="CB20" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC20" t="inlineStr">
+        <is>
+          <t>While both messages discuss the challenges of sentiment analysis in detecting sarcasm and irony, Message A provides a more detailed breakdown with examples and specific challenges, while Message B offers a more concise overview of the problem. Although there is overlap in the core theme, the level of detail and specific points differ significantly.</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5316,6 +6288,54 @@
       <c r="BO21" t="inlineStr"/>
       <c r="BP21" t="inlineStr"/>
       <c r="BQ21" t="inlineStr"/>
+      <c r="BR21" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS21" t="inlineStr">
+        <is>
+          <t>The response accurately covers key advancements in conversational AI and the future of human-AI interaction, providing detailed and factually correct information on various aspects such as natural language understanding, dialogue management, and ethical considerations.</t>
+        </is>
+      </c>
+      <c r="BT21" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU21" t="inlineStr">
+        <is>
+          <t>The response is well-structured, informative, and easy to follow, covering various aspects of advancements in conversational AI and their future implications clearly.</t>
+        </is>
+      </c>
+      <c r="BV21" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW21" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by discussing the advancements in conversational AI and the future of human-AI interaction in detail, covering various aspects such as technological improvements, impacts, and ethical considerations.</t>
+        </is>
+      </c>
+      <c r="BX21" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY21" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the advancements in conversational AI and the future of human-AI interaction, closely aligning with the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ21" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA21" t="inlineStr">
+        <is>
+          <t>The response offers a comprehensive and well-thought-out discussion of advancements in conversational AI, exploring both technical improvements and future implications, while also addressing ethical considerations, making it insightful and balanced.</t>
+        </is>
+      </c>
+      <c r="CB21" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC21" t="inlineStr">
+        <is>
+          <t>While Message A covers similar themes and advancements as Message B, it provides significantly more detail and specific examples, leading to a moderate variance in substance and meaning.</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5551,6 +6571,54 @@
       <c r="BO22" t="inlineStr"/>
       <c r="BP22" t="inlineStr"/>
       <c r="BQ22" t="inlineStr"/>
+      <c r="BR22" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS22" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and accurate overview of how AI systems should handle culturally sensitive topics in diverse environments, with practical strategies and acknowledgment of challenges.</t>
+        </is>
+      </c>
+      <c r="BT22" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU22" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, with clear sections and bullet points breaking down complex concepts effectively.</t>
+        </is>
+      </c>
+      <c r="BV22" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW22" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the prompt by detailing various strategies and considerations for AI systems to handle culturally sensitive topics in diverse environments.</t>
+        </is>
+      </c>
+      <c r="BX22" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY22" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the prompt's question, providing detailed and structured insights on how AI systems should handle culturally sensitive topics in diverse environments.</t>
+        </is>
+      </c>
+      <c r="BZ22" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA22" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and thoughtful approach to handling culturally sensitive topics in AI systems, demonstrating a deep understanding of the complexities involved and offering practical strategies for improvement.</t>
+        </is>
+      </c>
+      <c r="CB22" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC22" t="inlineStr">
+        <is>
+          <t>While Message A elaborates extensively on the same themes as Message B, including diverse datasets, contextual understanding, and ethical considerations, it introduces additional details and strategies that go beyond the scope of the benchmark, leading to a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5776,6 +6844,54 @@
       <c r="BO23" t="inlineStr"/>
       <c r="BP23" t="inlineStr"/>
       <c r="BQ23" t="inlineStr"/>
+      <c r="BR23" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS23" t="inlineStr">
+        <is>
+          <t>The response comprehensively and accurately outlines the challenges of translating idiomatic expressions across languages in NLP, covering key points like lack of direct equivalence, cultural relativity, limited resources, ambiguity, and the evolving nature of idioms, while also discussing solutions through NLP innovations.</t>
+        </is>
+      </c>
+      <c r="BT23" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU23" t="inlineStr">
+        <is>
+          <t>The response is highly clear and easy to understand, with well-structured points and examples that effectively communicate the challenges of translating idiomatic expressions in NLP.</t>
+        </is>
+      </c>
+      <c r="BV23" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW23" t="inlineStr">
+        <is>
+          <t>The response comprehensively discusses the challenges of translating idiomatic expressions across languages in NLP, addressing various aspects such as cultural relativity, context dependence, and the role of advanced NLP techniques.</t>
+        </is>
+      </c>
+      <c r="BX23" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY23" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the challenges of translating idiomatic expressions across languages in NLP, covering multiple aspects such as lack of direct equivalence, limited linguistic resources, ambiguous interpretations, and the evolving nature of idiomatic language, all while aligning perfectly with the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ23" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA23" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and well-structured exploration of the challenges in translating idiomatic expressions across languages in NLP, covering aspects such as cultural relativity, context dependence, and the role of advanced techniques like deep learning and context-aware embeddings.</t>
+        </is>
+      </c>
+      <c r="CB23" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC23" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and structured discussion, it aligns closely with the core ideas presented in Message B, addressing the challenges of translating idiomatic expressions due to cultural context, lack of direct equivalence, and the need for context-aware algorithms and diverse datasets.</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -6005,6 +7121,54 @@
       <c r="BO24" t="inlineStr"/>
       <c r="BP24" t="inlineStr"/>
       <c r="BQ24" t="inlineStr"/>
+      <c r="BR24" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS24" t="inlineStr">
+        <is>
+          <t>The response comprehensively and accurately explains the importance of cultural competence in AI language models, addressing key aspects such as avoiding bias, promoting meaningful communication, enhancing accessibility, and fostering ethical development.</t>
+        </is>
+      </c>
+      <c r="BT24" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU24" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, clearly outlining the importance of cultural competence in AI language models with examples and challenges.</t>
+        </is>
+      </c>
+      <c r="BV24" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW24" t="inlineStr">
+        <is>
+          <t>The response thoroughly addresses the prompt by detailing the importance of cultural competence in AI language models, covering aspects such as avoiding discrimination, promoting accurate communication, enhancing accessibility, and fostering ethical AI development.</t>
+        </is>
+      </c>
+      <c r="BX24" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY24" t="inlineStr">
+        <is>
+          <t>The response closely follows the prompt's instructions by thoroughly explaining the importance of cultural competence in AI language models, covering various aspects such as avoiding bias, promoting accurate communication, and fostering ethical AI development.</t>
+        </is>
+      </c>
+      <c r="BZ24" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA24" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and thoughtful exploration of cultural competence in AI language models, covering multiple dimensions such as avoiding bias, promoting accurate communication, enhancing accessibility, and fostering ethical development, while also acknowledging challenges and proposing solutions.</t>
+        </is>
+      </c>
+      <c r="CB24" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC24" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and structured explanation, it aligns closely with the core points presented in Message B, emphasizing the need for cultural competence to avoid bias, promote accurate communication, and foster inclusivity.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -6249,6 +7413,54 @@
       <c r="BO25" t="inlineStr"/>
       <c r="BP25" t="inlineStr"/>
       <c r="BQ25" t="inlineStr"/>
+      <c r="BR25" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS25" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and generally accurate outline for optimally scheduling tasks in a multiprocessor system, covering key concepts such as task decomposition, priority queues, and dynamic assignment. However, it could benefit from more precise details and specific algorithms for certain steps, such as local search methods for optimization, which slightly reduces the accuracy score.</t>
+        </is>
+      </c>
+      <c r="BT25" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU25" t="inlineStr">
+        <is>
+          <t>The response is well-structured and detailed, clearly outlining the steps of the algorithm and discussing important considerations, but it could benefit from more concise language and simpler explanations for some technical aspects.</t>
+        </is>
+      </c>
+      <c r="BV25" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW25" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by outlining a detailed algorithm for optimally scheduling tasks in a multiprocessor system to minimize total execution time.</t>
+        </is>
+      </c>
+      <c r="BX25" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY25" t="inlineStr">
+        <is>
+          <t>The response closely follows the prompt's instructions by developing an algorithm for optimally scheduling tasks in a multiprocessor system to minimize total execution time, covering relevant aspects such as problem definition, task decomposition, scheduling strategy, and optimization techniques.</t>
+        </is>
+      </c>
+      <c r="BZ25" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA25" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and well-structured approach to task scheduling in a multiprocessor system, demonstrating a good understanding of the problem and suggesting practical optimization strategies.</t>
+        </is>
+      </c>
+      <c r="CB25" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC25" t="inlineStr">
+        <is>
+          <t>Message A provides a detailed, step-by-step algorithm for task scheduling, while Message B offers a high-level overview of the key techniques involved. Although both messages address task scheduling in a multiprocessor system to minimize execution time, Message A includes specific strategies and implementation details that are not present in Message B, leading to a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -6483,6 +7695,54 @@
       <c r="BO26" t="inlineStr"/>
       <c r="BP26" t="inlineStr"/>
       <c r="BQ26" t="inlineStr"/>
+      <c r="BR26" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS26" t="inlineStr">
+        <is>
+          <t>The response thoroughly and accurately discusses the trade-offs between privacy and security in digital contact tracing systems, providing a detailed and balanced analysis of both aspects.</t>
+        </is>
+      </c>
+      <c r="BT26" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU26" t="inlineStr">
+        <is>
+          <t>The response is well-structured, comprehensive, and presents a clear analysis of the trade-offs between privacy and security in digital contact tracing systems, making it easy to understand.</t>
+        </is>
+      </c>
+      <c r="BV26" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW26" t="inlineStr">
+        <is>
+          <t>The response directly addresses the trade-offs between privacy and security in the design of digital contact tracing systems for pandemic response, thoroughly covering both aspects and their implications.</t>
+        </is>
+      </c>
+      <c r="BX26" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY26" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt, thoroughly analyzing the trade-offs between privacy and security in digital contact tracing systems, while also providing additional insights into ethical considerations and balancing these aspects.</t>
+        </is>
+      </c>
+      <c r="BZ26" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA26" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and balanced analysis of the trade-offs between privacy and security in digital contact tracing systems, offering detailed and thoughtful considerations for both aspects and suggesting practical solutions for finding equilibrium.</t>
+        </is>
+      </c>
+      <c r="CB26" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC26" t="inlineStr">
+        <is>
+          <t>Message A expands on the details provided in Message B but maintains a consistent focus on the trade-offs between privacy and security in digital contact tracing systems, with additional insights and specific measures to achieve balance.</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -6716,6 +7976,54 @@
       <c r="BO27" t="inlineStr"/>
       <c r="BP27" t="inlineStr"/>
       <c r="BQ27" t="inlineStr"/>
+      <c r="BR27" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS27" t="inlineStr">
+        <is>
+          <t>The response accurately outlines a comprehensive and multi-pronged strategy for mitigating the impact of deepfake technology, addressing prevention, detection, education, response, accountability, collaboration, and ethical considerations effectively.</t>
+        </is>
+      </c>
+      <c r="BT27" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU27" t="inlineStr">
+        <is>
+          <t>The response is highly detailed, well-structured, and easy to understand, presenting a clear and comprehensive strategy for mitigating the impact of deepfake technology.</t>
+        </is>
+      </c>
+      <c r="BV27" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW27" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by providing a comprehensive strategy for mitigating the impact of deepfake technology on the spread of misinformation and erosion of public trust, covering multiple aspects such as prevention, detection, response, accountability, collaboration, and ethical considerations.</t>
+        </is>
+      </c>
+      <c r="BX27" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY27" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the prompt by outlining a detailed strategy for mitigating the impact of deepfake technology on misinformation and public trust, covering technical, educational, legal, and ethical aspects.</t>
+        </is>
+      </c>
+      <c r="BZ27" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA27" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive, well-structured strategy for mitigating deepfakes, demonstrating a deep understanding of the issue and offering practical, multi-faceted solutions.</t>
+        </is>
+      </c>
+      <c r="CB27" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC27" t="inlineStr">
+        <is>
+          <t>While both messages address the issue of mitigating deepfakes and propose similar strategies, Message A provides significantly more detail and specific examples, leading to a moderate variance in substance and meaning.</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -6954,6 +8262,54 @@
       <c r="BO28" t="inlineStr"/>
       <c r="BP28" t="inlineStr"/>
       <c r="BQ28" t="inlineStr"/>
+      <c r="BR28" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS28" t="inlineStr">
+        <is>
+          <t>The response accurately addresses the prompt by outlining a comprehensive and sustainable urban transportation system that aims to minimize congestion and environmental impact while maximizing accessibility and equity.</t>
+        </is>
+      </c>
+      <c r="BT28" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU28" t="inlineStr">
+        <is>
+          <t>The response is exceptionally clear, providing a detailed and structured plan for a sustainable urban transportation system, with well-defined principles, components, and practices.</t>
+        </is>
+      </c>
+      <c r="BV28" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW28" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by detailing a comprehensive plan for a sustainable urban transportation system that minimizes congestion and environmental impact while maximizing accessibility and equity.</t>
+        </is>
+      </c>
+      <c r="BX28" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY28" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt by detailing a sustainable urban transportation system that minimizes congestion and environmental impact while maximizing accessibility and equity, with comprehensive coverage of key components and principles.</t>
+        </is>
+      </c>
+      <c r="BZ28" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA28" t="inlineStr">
+        <is>
+          <t>The response demonstrates a high level of insight by comprehensively addressing the prompt with a detailed, multifaceted approach to sustainable urban transportation that effectively balances minimizing congestion and environmental impact with maximizing accessibility and equity.</t>
+        </is>
+      </c>
+      <c r="CB28" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC28" t="inlineStr">
+        <is>
+          <t>While Message A provides more detailed and specific proposals, it closely aligns with the core principles and objectives outlined in Message B, focusing on multimodal integration, prioritizing public transit, promoting active transportation, and ensuring accessibility and equity.</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -7207,6 +8563,54 @@
       <c r="BO29" t="inlineStr"/>
       <c r="BP29" t="inlineStr"/>
       <c r="BQ29" t="inlineStr"/>
+      <c r="BR29" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS29" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and largely accurate breakdown of developing a machine learning model for predicting disease likelihood based on genetic and lifestyle factors, covering essential steps from data collection to deployment, with minor redundancies and slight specificity issues in certain steps.</t>
+        </is>
+      </c>
+      <c r="BT29" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU29" t="inlineStr">
+        <is>
+          <t>The response is highly detailed and well-organized, making it easy to follow the steps for developing the machine learning model, although some technical jargon might require background knowledge to fully understand.</t>
+        </is>
+      </c>
+      <c r="BV29" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW29" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by providing a detailed, step-by-step guide on developing a machine learning model for predicting disease likelihood based on genetic and lifestyle factors.</t>
+        </is>
+      </c>
+      <c r="BX29" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY29" t="inlineStr">
+        <is>
+          <t>The response perfectly adheres to the prompt's instructions by providing a detailed, structured plan for developing a machine learning model to predict the likelihood of a patient developing a specific disease based on their genetic and lifestyle factors.</t>
+        </is>
+      </c>
+      <c r="BZ29" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA29" t="inlineStr">
+        <is>
+          <t>The response demonstrates a deep understanding of the complex process of developing a machine learning model for disease prediction, including detailed steps for data collection, feature engineering, model selection, and ethical considerations, providing a comprehensive and thoughtful approach.</t>
+        </is>
+      </c>
+      <c r="CB29" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC29" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and comprehensive breakdown of the process compared to Message B, the core substance and meaning remain aligned. Both messages address data collection, feature engineering, model training, and clinical application, but Message A includes additional specifics and steps.</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -7439,6 +8843,54 @@
       <c r="BO30" t="inlineStr"/>
       <c r="BP30" t="inlineStr"/>
       <c r="BQ30" t="inlineStr"/>
+      <c r="BR30" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS30" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and accurate explanation of quantum entanglement and its potential applications in cryptography and computing, with only minor simplifications that do not detract from its overall correctness.</t>
+        </is>
+      </c>
+      <c r="BT30" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU30" t="inlineStr">
+        <is>
+          <t>The response is well-structured and effectively explains quantum entanglement and its applications in cryptography and computing, though some sections could be simplified for broader accessibility.</t>
+        </is>
+      </c>
+      <c r="BV30" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW30" t="inlineStr">
+        <is>
+          <t>The response thoroughly explains the concept of quantum entanglement and its applications in cryptography and computing, directly addressing the prompt with only a minor inclusion of additional context that remains relevant.</t>
+        </is>
+      </c>
+      <c r="BX30" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY30" t="inlineStr">
+        <is>
+          <t>The response thoroughly explains the concept of quantum entanglement and its potential applications in cryptography and computing, closely aligning with the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ30" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA30" t="inlineStr">
+        <is>
+          <t>The response provides a clear and comprehensive explanation of quantum entanglement, its applications in cryptography and computing, and its future potential, demonstrating a solid understanding and thoughtful exploration of the topic.</t>
+        </is>
+      </c>
+      <c r="CB30" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC30" t="inlineStr">
+        <is>
+          <t>While Message A provides more detailed explanations and examples, it retains the core concepts and applications of quantum entanglement as described in Message B, resulting in a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -7654,6 +9106,54 @@
       <c r="BO31" t="inlineStr"/>
       <c r="BP31" t="inlineStr"/>
       <c r="BQ31" t="inlineStr"/>
+      <c r="BR31" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS31" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and mostly accurate overview of the roles of dark matter and dark energy in the universe's structure and evolution, with only minor inaccuracies and simplifications.</t>
+        </is>
+      </c>
+      <c r="BT31" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU31" t="inlineStr">
+        <is>
+          <t>The response is very well-structured and detailed, providing a clear and thorough explanation of the roles of dark matter and dark energy in the universe's structure and evolution.</t>
+        </is>
+      </c>
+      <c r="BV31" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW31" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the role of dark matter and dark energy in the universe's structure and evolution, directly aligning with the prompt.</t>
+        </is>
+      </c>
+      <c r="BX31" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY31" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the role of dark matter and dark energy in the universe's structure and evolution, closely adhering to the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ31" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA31" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive, well-structured explanation of dark matter and dark energy, demonstrating a strong understanding of their roles and the current scientific challenges, making it highly insightful.</t>
+        </is>
+      </c>
+      <c r="CB31" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC31" t="inlineStr">
+        <is>
+          <t>While both messages convey the fundamental roles of dark matter and dark energy, Message A provides significantly more detail and additional aspects such as gravitational lensing and challenges in detection, which are not present in Message B, leading to a moderate variance.</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -7876,6 +9376,54 @@
       <c r="BO32" t="inlineStr"/>
       <c r="BP32" t="inlineStr"/>
       <c r="BQ32" t="inlineStr"/>
+      <c r="BR32" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS32" t="inlineStr">
+        <is>
+          <t>The response accurately outlines the major challenges and potential benefits of developing artificial general intelligence (AGI), covering a wide range of relevant points.</t>
+        </is>
+      </c>
+      <c r="BT32" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU32" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, clearly outlining both the challenges and benefits of developing AGI.</t>
+        </is>
+      </c>
+      <c r="BV32" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW32" t="inlineStr">
+        <is>
+          <t>The response comprehensively addresses the challenges and potential benefits of developing artificial general intelligence (AGI), aligning perfectly with the prompt.</t>
+        </is>
+      </c>
+      <c r="BX32" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY32" t="inlineStr">
+        <is>
+          <t>The response thoroughly addresses both the challenges and potential benefits of developing artificial general intelligence (AGI), aligning perfectly with the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ32" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA32" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and thoughtful exploration of the challenges and benefits of developing AGI, demonstrating a deep understanding of the topic and offering balanced perspectives on its potential impact.</t>
+        </is>
+      </c>
+      <c r="CB32" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC32" t="inlineStr">
+        <is>
+          <t>While both messages discuss the challenges and benefits of developing AGI, Message A provides a more detailed breakdown and includes specific examples and ethical considerations that are not fully covered in Message B, leading to a moderate level of variance.</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -8096,6 +9644,54 @@
       <c r="BO33" t="inlineStr"/>
       <c r="BP33" t="inlineStr"/>
       <c r="BQ33" t="inlineStr"/>
+      <c r="BR33" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS33" t="inlineStr">
+        <is>
+          <t>The response accurately explains the concept of neuroplasticity and its implications for learning, memory, and recovery from brain injuries, though it slightly exaggerates the extent to which the brain can grow new neurons, which is more limited than implied.</t>
+        </is>
+      </c>
+      <c r="BT33" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU33" t="inlineStr">
+        <is>
+          <t>The response is well-structured, thorough, and easy to understand, effectively explaining neuroplasticity and its implications with clear examples and practical advice.</t>
+        </is>
+      </c>
+      <c r="BV33" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW33" t="inlineStr">
+        <is>
+          <t>The response comprehensively explains neuroplasticity and its implications for learning, memory, and recovery from brain injuries, directly addressing all aspects of the prompt.</t>
+        </is>
+      </c>
+      <c r="BX33" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY33" t="inlineStr">
+        <is>
+          <t>The response comprehensively explains neuroplasticity and effectively addresses its implications for learning, memory, and recovery from brain injuries, closely adhering to the prompt's instructions.</t>
+        </is>
+      </c>
+      <c r="BZ33" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA33" t="inlineStr">
+        <is>
+          <t>The response provides a detailed, accurate, and engaging explanation of neuroplasticity, effectively highlighting its implications for learning, memory, and recovery from brain injuries, and offering practical advice for enhancing neuroplasticity.</t>
+        </is>
+      </c>
+      <c r="CB33" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC33" t="inlineStr">
+        <is>
+          <t>While Message A provides a more detailed and expansive explanation of neuroplasticity with additional examples and implications, it retains the core substance and meaning of Message B, focusing on the brain's ability to change, its impact on learning, memory, and recovery from brain injuries. However, the extra details and structural differences warrant a moderate variance rating.</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -8320,6 +9916,54 @@
       <c r="BO34" t="inlineStr"/>
       <c r="BP34" t="inlineStr"/>
       <c r="BQ34" t="inlineStr"/>
+      <c r="BR34" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS34" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and largely accurate description of the Rabbit R1 server, highlighting its hardware specifications, liquid cooling system, networking capabilities, and other features, which aligns well with known information about the server.</t>
+        </is>
+      </c>
+      <c r="BT34" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU34" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, clearly explaining the features and capabilities of the Rabbit R1 server.</t>
+        </is>
+      </c>
+      <c r="BV34" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW34" t="inlineStr">
+        <is>
+          <t>The response is entirely focused on explaining the Rabbit R1, providing detailed and relevant information about its features, capabilities, and intended use cases.</t>
+        </is>
+      </c>
+      <c r="BX34" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY34" t="inlineStr">
+        <is>
+          <t>The response perfectly adheres to the prompt by providing a comprehensive and detailed explanation of what the Rabbit R1 is.</t>
+        </is>
+      </c>
+      <c r="BZ34" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA34" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and comprehensive overview of the Rabbit R1 server, showcasing a good understanding of its technical specifications and applications, but it lacks deeper analysis or unique insights beyond the factual information.</t>
+        </is>
+      </c>
+      <c r="CB34" t="n">
+        <v>10</v>
+      </c>
+      <c r="CC34" t="inlineStr">
+        <is>
+          <t>The two messages diverge completely in substance and meaning; Message A describes a high-performance server designed for cloud computing and AI, while Message B describes a personal assistant device with voice command and touch interaction features. There is no overlap in the content, warranting the highest possible variance rating.</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -8535,6 +10179,54 @@
       <c r="BO35" t="inlineStr"/>
       <c r="BP35" t="inlineStr"/>
       <c r="BQ35" t="inlineStr"/>
+      <c r="BR35" t="n">
+        <v>7</v>
+      </c>
+      <c r="BS35" t="inlineStr">
+        <is>
+          <t>While the response provides a detailed and mostly accurate overview of Naval Ravikant's background and contributions, it contains a notable inaccuracy: Naval Ravikant is not the author of "Mastering Bitcoin." Additionally, the podcast "Reply All" is not associated with Naval Ravikant. These errors slightly reduce the overall accuracy of the response.</t>
+        </is>
+      </c>
+      <c r="BT35" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU35" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a comprehensive overview of Naval Ravikant's background and ideas, making it easy to understand, although some details could be more concise.</t>
+        </is>
+      </c>
+      <c r="BV35" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW35" t="inlineStr">
+        <is>
+          <t>The response provides detailed and accurate information about Naval Ravikant, covering his professional background, contributions, and philosophies, directly addressing the prompt's question.</t>
+        </is>
+      </c>
+      <c r="BX35" t="n">
+        <v>6</v>
+      </c>
+      <c r="BY35" t="inlineStr">
+        <is>
+          <t>While the response provides extensive information about Naval Ravikant, it includes details that go beyond the scope of the simple prompt, which only asks for an identification of who he is.</t>
+        </is>
+      </c>
+      <c r="BZ35" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA35" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and well-structured overview of Naval Ravikant's career and philosophies, offering a balanced and insightful summary that goes beyond basic information.</t>
+        </is>
+      </c>
+      <c r="CB35" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC35" t="inlineStr">
+        <is>
+          <t>While Message A and Message B share many similarities in substance and meaning, Message A introduces additional details and some inaccuracies, such as incorrectly attributing the book "Mastering Bitcoin" and the podcast "Reply All" to Naval Ravikant, which increases the variance slightly.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -8770,6 +10462,54 @@
       <c r="BO36" t="inlineStr"/>
       <c r="BP36" t="inlineStr"/>
       <c r="BQ36" t="inlineStr"/>
+      <c r="BR36" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS36" t="inlineStr">
+        <is>
+          <t>The response accurately reflects the prompt's description of a future Earth with different factions planning for long-distance space travel to establish societies on exoplanets, and the personal struggle of choosing a faction, without using the words 'testament' or 'tapestry'.</t>
+        </is>
+      </c>
+      <c r="BT36" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU36" t="inlineStr">
+        <is>
+          <t>The response is well-written and presents a clear narrative, effectively introducing the main character, the central conflict, and the three factions, making it easy to understand the premise of the story.</t>
+        </is>
+      </c>
+      <c r="BV36" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW36" t="inlineStr">
+        <is>
+          <t>The response is highly relevant to the prompt, effectively introducing the setting, the space race, the different factions, and the weight of the decision individuals must make for future generations.</t>
+        </is>
+      </c>
+      <c r="BX36" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY36" t="inlineStr">
+        <is>
+          <t>The response closely follows the prompt's instructions, introducing the main theme of the book, the three factions, and the protagonist's dilemma, while avoiding the use of the words 'testament' and 'tapestry', although it could be slightly more engaging from the very beginning.</t>
+        </is>
+      </c>
+      <c r="BZ36" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA36" t="inlineStr">
+        <is>
+          <t>The response effectively explores the complexities and moral dilemmas of the prompt, demonstrating a thoughtful consideration of the different factions and their philosophies, and the profound impact of the decision on future generations.</t>
+        </is>
+      </c>
+      <c r="CB36" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC36" t="inlineStr">
+        <is>
+          <t>While both messages convey the theme of choosing between different factions for interstellar colonization, there are notable differences in character names, setting details, the number and names of factions, and the specific philosophies they represent. However, the core dilemma and the need to choose a future for subsequent generations are present in both, indicating a moderate level of variance.</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -8994,6 +10734,54 @@
       <c r="BO37" t="inlineStr"/>
       <c r="BP37" t="inlineStr"/>
       <c r="BQ37" t="inlineStr"/>
+      <c r="BR37" t="n">
+        <v>5</v>
+      </c>
+      <c r="BS37" t="inlineStr">
+        <is>
+          <t>The response provides a detailed explanation of a well-being approach but incorrectly identifies what SPIRE stands for and its components. The actual SPIRE method stands for Spiritual, Physical, Intellectual, Relational, and Emotional well-being.</t>
+        </is>
+      </c>
+      <c r="BT37" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU37" t="inlineStr">
+        <is>
+          <t>The response is well-structured, comprehensive, and easy to understand, providing a clear explanation of the SPIRE method, its components, and how to carry out a SPIRE check-in.</t>
+        </is>
+      </c>
+      <c r="BV37" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW37" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by explaining the 'SPIRE' method, what it stands for, and how to carry out a SPIRE check-in in detail.</t>
+        </is>
+      </c>
+      <c r="BX37" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY37" t="inlineStr">
+        <is>
+          <t>The response perfectly adheres to the prompt, thoroughly explaining the 'SPIRE' method for holistic well-being, what 'SPIRE' stands for, and how to carry out a SPIRE check-in.</t>
+        </is>
+      </c>
+      <c r="BZ37" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA37" t="inlineStr">
+        <is>
+          <t>The response provides a thorough and well-structured explanation of the SPIRE method, offering detailed insights into each component and practical steps for carrying out a SPIRE check-in, making it both informative and thoughtful.</t>
+        </is>
+      </c>
+      <c r="CB37" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC37" t="inlineStr">
+        <is>
+          <t>While both messages discuss a holistic well-being approach called SPIRE, the acronym and its components differ significantly, with Message A focusing on Strengths, Positive changes, Improve self-care, Relationships, and Enjoyment, and Message B on Spiritual, Physical, Intellectual, Relational, and Emotional aspects. However, they share the common goal of reflecting on various life aspects for overall well-being, resulting in a moderate variance rating.</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -9217,6 +11005,54 @@
       <c r="BO38" t="inlineStr"/>
       <c r="BP38" t="inlineStr"/>
       <c r="BQ38" t="inlineStr"/>
+      <c r="BR38" t="n">
+        <v>7</v>
+      </c>
+      <c r="BS38" t="inlineStr">
+        <is>
+          <t>The response is mostly accurate, providing a good overview of Wing Chun's origins, characteristics, and impact, but it contains some inaccuracies, such as the inclusion of "Drunken Fist" and the emphasis on internal energy cultivation, which are not central to Wing Chun.</t>
+        </is>
+      </c>
+      <c r="BT38" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU38" t="inlineStr">
+        <is>
+          <t>The response is highly clear and easy to understand, providing a structured explanation of Wing Chun, its origins, characteristics, principles, impact, and how to learn it.</t>
+        </is>
+      </c>
+      <c r="BV38" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW38" t="inlineStr">
+        <is>
+          <t>The response comprehensively and directly addresses the prompt, providing detailed information about Wing Chun, its origins, characteristics, principles, impact, and how to learn it.</t>
+        </is>
+      </c>
+      <c r="BX38" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY38" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed explanation of Wing Chun, closely adhering to the prompt's request for information about 'Wing Chun', although it includes some extraneous details that go beyond a concise definition.</t>
+        </is>
+      </c>
+      <c r="BZ38" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA38" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and detailed overview of Wing Chun, including its origins, characteristics, principles, and impact, demonstrating a good level of insight into the martial art.</t>
+        </is>
+      </c>
+      <c r="CB38" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC38" t="inlineStr">
+        <is>
+          <t>While both messages describe Wing Chun as a Chinese martial art with a focus on close-range combat and efficient movements, Message A introduces additional historical context, specific techniques, and cultural impact that are not present in Message B, leading to a moderate level of variance.</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -9443,6 +11279,54 @@
       <c r="BO39" t="inlineStr"/>
       <c r="BP39" t="inlineStr"/>
       <c r="BQ39" t="inlineStr"/>
+      <c r="BR39" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS39" t="inlineStr">
+        <is>
+          <t>The response provides a mostly accurate depiction of Morihei Ueshiba, his role as the founder of Aikido, and his spiritual teachings; however, it contains a minor inaccuracy regarding his birth year, which should be 1883 instead of 1904.</t>
+        </is>
+      </c>
+      <c r="BT39" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU39" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a detailed and easy-to-understand overview of Morihei Ueshiba's life, contributions, and legacy, though the length and depth might be more than necessary for a simple prompt.</t>
+        </is>
+      </c>
+      <c r="BV39" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW39" t="inlineStr">
+        <is>
+          <t>The response is directly relevant to the prompt, providing detailed and accurate information about Morihei Ueshiba, his role as the founder of Aikido, and his spiritual teachings.</t>
+        </is>
+      </c>
+      <c r="BX39" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY39" t="inlineStr">
+        <is>
+          <t>The response provides detailed and relevant information about Morihei Ueshiba, his contributions to martial arts, and his spiritual teachings, closely aligning with the prompt's request for information about him.</t>
+        </is>
+      </c>
+      <c r="BZ39" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA39" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and thoughtful exploration of Morihei Ueshiba's life and the principles of Aikido, offering a balanced perspective on his contributions to martial arts and spiritual teaching, although it could benefit from more unique or personal insights.</t>
+        </is>
+      </c>
+      <c r="CB39" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC39" t="inlineStr">
+        <is>
+          <t>While Message A provides more detail and elaborates on certain aspects of Morihei Ueshiba's life and teachings, the core substance and meaning align closely with Message B, focusing on his role as the founder of Aikido, his emphasis on harmony and spiritual growth, and his influence in the martial arts community.</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -9659,6 +11543,54 @@
       <c r="BO40" t="inlineStr"/>
       <c r="BP40" t="inlineStr"/>
       <c r="BQ40" t="inlineStr"/>
+      <c r="BR40" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS40" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and largely accurate depiction of Miyamoto Musashi's life and accomplishments, but includes a few minor inaccuracies and exaggerations, such as the claim that his duel with Sasaki Kojiro ended in mutual respect and admiration, which is not historically documented.</t>
+        </is>
+      </c>
+      <c r="BT40" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU40" t="inlineStr">
+        <is>
+          <t>The response is well-structured, detailed, and easy to understand, providing a comprehensive overview of Miyamoto Musashi's life and legacy.</t>
+        </is>
+      </c>
+      <c r="BV40" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW40" t="inlineStr">
+        <is>
+          <t>The response is entirely focused on Miyamoto Musashi, providing detailed and relevant information about his life, skills, historical significance, and cultural impact, which is exactly what the prompt asks for.</t>
+        </is>
+      </c>
+      <c r="BX40" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY40" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and comprehensive overview of Miyamoto Musashi's life, skills, historical significance, and literary legacy, closely aligning with the prompt's request for information about who he was.</t>
+        </is>
+      </c>
+      <c r="BZ40" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA40" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive overview of Miyamoto Musashi's life, skills, and legacy, demonstrating a good understanding of his historical significance and cultural impact.</t>
+        </is>
+      </c>
+      <c r="CB40" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC40" t="inlineStr">
+        <is>
+          <t>While both messages convey similar overarching themes about Miyamoto Musashi's renown as a swordsman, philosopher, and author of "The Book of Five Rings," Message A provides significantly more detailed and somewhat fictionalized narrative elements, leading to a moderate level of variance in substance and meaning.</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -9883,6 +11815,54 @@
       <c r="BO41" t="inlineStr"/>
       <c r="BP41" t="inlineStr"/>
       <c r="BQ41" t="inlineStr"/>
+      <c r="BR41" t="n">
+        <v>7</v>
+      </c>
+      <c r="BS41" t="inlineStr">
+        <is>
+          <t>While the response provides a detailed overview of "The Book of Five Rings" and its author Miyamoto Musashi, it includes some misleading interpretations of the book's content and the historical context of its publication.</t>
+        </is>
+      </c>
+      <c r="BT41" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU41" t="inlineStr">
+        <is>
+          <t>While the response provides a detailed and well-structured explanation, the inclusion of additional sections like "Influence" and "Beyond Warfare" can be distracting from the direct prompt, and the use of non-standard terms for the "rings" may cause some confusion.</t>
+        </is>
+      </c>
+      <c r="BV41" t="n">
+        <v>7</v>
+      </c>
+      <c r="BW41" t="inlineStr">
+        <is>
+          <t>The response provides relevant information about 'The Book of Five Rings', its author Miyamoto Musashi, and its content, but it includes excessive detail and additional context that goes beyond the direct scope of the prompt.</t>
+        </is>
+      </c>
+      <c r="BX41" t="n">
+        <v>7</v>
+      </c>
+      <c r="BY41" t="inlineStr">
+        <is>
+          <t>The response addresses the core of the prompt by identifying the book, its author, and providing a detailed explanation of its content, but it fails to provide a precise first publication date and includes excessive additional information not requested in the prompt.</t>
+        </is>
+      </c>
+      <c r="BZ41" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA41" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and thoughtful exploration of "The Book of Five Rings," breaking down the five principles and their applications beyond warfare, showcasing a deep understanding and insightful interpretation of the text.</t>
+        </is>
+      </c>
+      <c r="CB41" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC41" t="inlineStr">
+        <is>
+          <t>While both messages identify Miyamoto Musashi as the author and discuss the book's strategic themes, Message A introduces different "rings" or principles that deviate from the original elements (Earth, Water, Fire, Wind, Void) described in Message B, leading to a moderate level of variance.</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -10105,6 +12085,54 @@
       <c r="BO42" t="inlineStr"/>
       <c r="BP42" t="inlineStr"/>
       <c r="BQ42" t="inlineStr"/>
+      <c r="BR42" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS42" t="inlineStr">
+        <is>
+          <t>The response accurately identifies and discusses various aspects of life without verbal or written language, including changes in communication, societal structures, and challenges, although some points are speculative, they are largely reasonable and well-considered.</t>
+        </is>
+      </c>
+      <c r="BT42" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU42" t="inlineStr">
+        <is>
+          <t>The response is well-structured and easy to understand, with clear points and detailed explanations, though some sections could be simplified for better readability.</t>
+        </is>
+      </c>
+      <c r="BV42" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW42" t="inlineStr">
+        <is>
+          <t>The response is entirely focused on the prompt, thoroughly exploring various aspects of a world without verbal or written language and its impacts on society, culture, and human interaction.</t>
+        </is>
+      </c>
+      <c r="BX42" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY42" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt by detailing various aspects of life without verbal or written language, although it goes beyond the basic requirements by offering extensive elaboration and speculative scenarios.</t>
+        </is>
+      </c>
+      <c r="BZ42" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA42" t="inlineStr">
+        <is>
+          <t>The response demonstrates a high level of insight by exploring various facets of human communication, society, and culture, and considering both the challenges and potential solutions in a world without language.</t>
+        </is>
+      </c>
+      <c r="CB42" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC42" t="inlineStr">
+        <is>
+          <t>Message A provides a more detailed and extensive exploration of the implications of a world without verbal or written language, offering specific examples and societal impacts, while Message B offers a more concise overview focusing on communication methods and general societal development. They share the core idea but differ in depth and specific points discussed.</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -10324,6 +12352,54 @@
       <c r="BO43" t="inlineStr"/>
       <c r="BP43" t="inlineStr"/>
       <c r="BQ43" t="inlineStr"/>
+      <c r="BR43" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS43" t="inlineStr">
+        <is>
+          <t>The response accurately describes the Fediverse, its decentralized nature, key features, popular platforms, and advantages, with only minor omissions that do not detract from its overall correctness.</t>
+        </is>
+      </c>
+      <c r="BT43" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU43" t="inlineStr">
+        <is>
+          <t>The response is well-structured, informative, and easy to understand, clearly explaining the concept of the Fediverse, its features, and advantages.</t>
+        </is>
+      </c>
+      <c r="BV43" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW43" t="inlineStr">
+        <is>
+          <t>The response is entirely focused on explaining the Fediverse, covering its definition, how it works, key features, popular platforms, advantages, and future prospects, making it fully relevant to the prompt.</t>
+        </is>
+      </c>
+      <c r="BX43" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY43" t="inlineStr">
+        <is>
+          <t>The response comprehensively answers the prompt by explaining what the Fediverse is, detailing its structure, features, and advantages, while also providing examples of popular platforms within it.</t>
+        </is>
+      </c>
+      <c r="BZ43" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA43" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and well-articulated explanation of the Fediverse, highlighting its key features, advantages, and popular platforms, demonstrating both depth and clarity.</t>
+        </is>
+      </c>
+      <c r="CB43" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC43" t="inlineStr">
+        <is>
+          <t>While Message A provides significantly more detail and examples, it maintains the core substance and meaning of Message B, explaining the Fediverse as a network of interconnected communities using shared protocols and emphasizing user control and privacy.</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -10546,6 +12622,54 @@
       <c r="BO44" t="inlineStr"/>
       <c r="BP44" t="inlineStr"/>
       <c r="BQ44" t="inlineStr"/>
+      <c r="BR44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS44" t="inlineStr">
+        <is>
+          <t>The response describes "Walden" by Henry David Thoreau instead of the book "Walking," which is a completely different work by the same author.</t>
+        </is>
+      </c>
+      <c r="BT44" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU44" t="inlineStr">
+        <is>
+          <t>The response is well-structured and provides a detailed explanation of Thoreau's views, but it mistakenly refers to "Walden" instead of "Walking," which slightly decreases its clarity in relation to the prompt.</t>
+        </is>
+      </c>
+      <c r="BV44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW44" t="inlineStr">
+        <is>
+          <t>The response discusses "Walden" by Henry David Thoreau, not "Walking," and is therefore mostly irrelevant to the prompt.</t>
+        </is>
+      </c>
+      <c r="BX44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY44" t="inlineStr">
+        <is>
+          <t>The response completely disregards the prompt by discussing "Walden" instead of "Walking" by Henry David Thoreau.</t>
+        </is>
+      </c>
+      <c r="BZ44" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA44" t="inlineStr">
+        <is>
+          <t>The response provides a detailed and thoughtful exploration of Thoreau's "Walden," highlighting key themes and offering a nuanced understanding of the book's essence, although it mistakenly refers to "Walking" as "Walden."</t>
+        </is>
+      </c>
+      <c r="CB44" t="n">
+        <v>9</v>
+      </c>
+      <c r="CC44" t="inlineStr">
+        <is>
+          <t>Message A discusses "Walden" and its themes of simplicity, self-reliance, and connection to nature, while Message B focuses on "Walking" and its emphasis on the spiritual and liberating act of walking in nature, resulting in a high variance due to the discussion of entirely different works and their respective themes.</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -10790,6 +12914,54 @@
       <c r="BO45" t="inlineStr"/>
       <c r="BP45" t="inlineStr"/>
       <c r="BQ45" t="inlineStr"/>
+      <c r="BR45" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS45" t="inlineStr">
+        <is>
+          <t>The response provides a detailed, accurate, and safe workout plan tailored to the individual's needs, including warm-ups, cool-downs, and important considerations for a balanced fitness routine.</t>
+        </is>
+      </c>
+      <c r="BT45" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU45" t="inlineStr">
+        <is>
+          <t>The response is highly clear and detailed, with a step-by-step workout plan that is easy to understand and follow, including specific exercises, sets, and repetitions for each week.</t>
+        </is>
+      </c>
+      <c r="BV45" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW45" t="inlineStr">
+        <is>
+          <t>The response provides a detailed weekly workout plan that targets different muscle groups and areas of physical fitness, directly addressing the prompt's requirements for a 38-year-old male getting back into exercise.</t>
+        </is>
+      </c>
+      <c r="BX45" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY45" t="inlineStr">
+        <is>
+          <t>The response provides a detailed weekly workout plan tailored to a 38-year-old male, focusing on different muscle groups and areas of fitness each week, with practical advice and clear instructions, fully adhering to the prompt.</t>
+        </is>
+      </c>
+      <c r="BZ45" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA45" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and well-structured weekly workout plan, including warm-ups, cool-downs, and detailed exercises for different muscle groups, demonstrating a good understanding of fitness principles.</t>
+        </is>
+      </c>
+      <c r="CB45" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC45" t="inlineStr">
+        <is>
+          <t>While both messages provide a weekly workout plan, Message A includes detailed warm-up and cool-down instructions, safety considerations, and progressive guidelines, whereas Message B focuses solely on the exercises and reps for each week without additional context or safety advice.</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -11013,6 +13185,54 @@
       <c r="BO46" t="inlineStr"/>
       <c r="BP46" t="inlineStr"/>
       <c r="BQ46" t="inlineStr"/>
+      <c r="BR46" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS46" t="inlineStr">
+        <is>
+          <t>The response provides a thorough, factual, and accurate explanation of the conflicts of interest big tech companies face regarding customer data, detailing revenue generation, business model focus, lack of transparency, competition dynamics, and regulatory challenges.</t>
+        </is>
+      </c>
+      <c r="BT46" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU46" t="inlineStr">
+        <is>
+          <t>The response is well-structured and detailed, providing a clear breakdown of the issues surrounding big tech companies and customer data, although it could be slightly more concise to enhance readability.</t>
+        </is>
+      </c>
+      <c r="BV46" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW46" t="inlineStr">
+        <is>
+          <t>The response thoroughly addresses the prompt by detailing the conflict of interest big tech companies face when handling customer data, including revenue generation, business model focus, lack of transparency, competition dynamics, and regulatory challenges, all of which are directly relevant to the prompt.</t>
+        </is>
+      </c>
+      <c r="BX46" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY46" t="inlineStr">
+        <is>
+          <t>The response thoroughly addresses the prompt by detailing the conflicts of interest that arise from big tech companies leveraging customer data, although it slightly deviates by also discussing regulatory challenges and ethical practices.</t>
+        </is>
+      </c>
+      <c r="BZ46" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA46" t="inlineStr">
+        <is>
+          <t>The response provides a comprehensive and well-structured analysis of the complex dynamics and conflicts of interest involved in how big tech companies handle customer data, offering a balanced perspective on both the challenges and the potential solutions.</t>
+        </is>
+      </c>
+      <c r="CB46" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC46" t="inlineStr">
+        <is>
+          <t>While Message A expands on the benchmark's points with detailed examples and additional context, it maintains the core argument about the conflict of interest and lack of trust in big tech companies handling user data. However, the length and detail in Message A introduce some divergence from the concise and direct approach of Message B.</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -11226,6 +13446,54 @@
       <c r="BO47" t="inlineStr"/>
       <c r="BP47" t="inlineStr"/>
       <c r="BQ47" t="inlineStr"/>
+      <c r="BR47" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS47" t="inlineStr">
+        <is>
+          <t>The response effectively captures the atmosphere and internal struggle of the narrator from 'Fight Club', continuing the story with a plausible exploration of the character's mental state after the events of the novel.</t>
+        </is>
+      </c>
+      <c r="BT47" t="n">
+        <v>8</v>
+      </c>
+      <c r="BU47" t="inlineStr">
+        <is>
+          <t>The response is well-structured and effectively conveys the narrator's internal struggle, with vivid descriptions and clear progression of thoughts, although some metaphorical language may require deeper interpretation.</t>
+        </is>
+      </c>
+      <c r="BV47" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW47" t="inlineStr">
+        <is>
+          <t>The response directly continues the narrative from the end of 'Fight Club,' exploring The Narrator's struggle with Tyler's lingering influence, which is highly relevant to the prompt.</t>
+        </is>
+      </c>
+      <c r="BX47" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY47" t="inlineStr">
+        <is>
+          <t>The response closely adheres to the prompt by picking up the story right after the end of the original novel, maintaining the tone and themes of 'Fight Club,' and effectively exploring the lingering presence of Tyler in The Narrator's mind.</t>
+        </is>
+      </c>
+      <c r="BZ47" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA47" t="inlineStr">
+        <is>
+          <t>The response effectively captures the psychological turmoil and lingering presence of Tyler, offering a nuanced exploration of the narrator's internal struggle and setting the stage for a compelling continuation of the story.</t>
+        </is>
+      </c>
+      <c r="CB47" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC47" t="inlineStr">
+        <is>
+          <t>While both messages convey the lingering presence of Tyler, Message A expands on the Narrator's internal struggle and the void left by Tyler's absence, whereas Message B focuses more on the immediate realization that Tyler is not gone. There is some overlap in theme, but the substance and specific details differ significantly.</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -11432,6 +13700,54 @@
       <c r="BO48" t="inlineStr"/>
       <c r="BP48" t="inlineStr"/>
       <c r="BQ48" t="inlineStr"/>
+      <c r="BR48" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS48" t="inlineStr">
+        <is>
+          <t>The response is completely factually correct, accurately explaining the blue color of the sky due to Rayleigh scattering.</t>
+        </is>
+      </c>
+      <c r="BT48" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU48" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear, concise, and easy to understand, with a straightforward explanation of why the sky appears blue.</t>
+        </is>
+      </c>
+      <c r="BV48" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW48" t="inlineStr">
+        <is>
+          <t>The response directly addresses the color of the sky on a clear day and provides relevant scientific explanation, making it highly relevant to the prompt.</t>
+        </is>
+      </c>
+      <c r="BX48" t="n">
+        <v>7</v>
+      </c>
+      <c r="BY48" t="inlineStr">
+        <is>
+          <t>The response correctly identifies the color of the sky on a clear day as blue but provides additional scientific explanation which, while informative, goes beyond the direct simplicity requested by the prompt.</t>
+        </is>
+      </c>
+      <c r="BZ48" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA48" t="inlineStr">
+        <is>
+          <t>The response provides a clear and detailed scientific explanation of why the sky appears blue, demonstrating a good understanding of the underlying phenomenon and offering insight beyond a simple answer.</t>
+        </is>
+      </c>
+      <c r="CB48" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC48" t="inlineStr">
+        <is>
+          <t>While Message A provides additional details on the scientific reason for the sky's color, the core substance and meaning—that the sky is blue on a clear day—remain consistent with Message B.</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -11635,6 +13951,54 @@
       <c r="BO49" t="inlineStr"/>
       <c r="BP49" t="inlineStr"/>
       <c r="BQ49" t="inlineStr"/>
+      <c r="BR49" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS49" t="inlineStr">
+        <is>
+          <t>The response correctly states that Christmas is celebrated on December 25th and accurately describes common traditions associated with the holiday.</t>
+        </is>
+      </c>
+      <c r="BT49" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU49" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, providing a straightforward answer to the prompt and additional context about the celebration.</t>
+        </is>
+      </c>
+      <c r="BV49" t="n">
+        <v>9</v>
+      </c>
+      <c r="BW49" t="inlineStr">
+        <is>
+          <t>The response directly answers the prompt by stating the date of Christmas and adds relevant details about its customs.</t>
+        </is>
+      </c>
+      <c r="BX49" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY49" t="inlineStr">
+        <is>
+          <t>The response accurately answers the question about when Christmas is but includes additional information that was not specifically requested.</t>
+        </is>
+      </c>
+      <c r="BZ49" t="n">
+        <v>3</v>
+      </c>
+      <c r="CA49" t="inlineStr">
+        <is>
+          <t>The response provides basic factual information about Christmas but lacks depth or unique perspective, making it unoriginal and not particularly insightful.</t>
+        </is>
+      </c>
+      <c r="CB49" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC49" t="inlineStr">
+        <is>
+          <t>While Message A includes additional context about Christmas traditions, it accurately conveys the date of December 25th, which is the primary information in Message B.</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -11834,6 +14198,54 @@
       <c r="BO50" t="inlineStr"/>
       <c r="BP50" t="inlineStr"/>
       <c r="BQ50" t="inlineStr"/>
+      <c r="BR50" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS50" t="inlineStr">
+        <is>
+          <t>The response correctly states that the entity is a language model and does not have a gender, which is entirely accurate.</t>
+        </is>
+      </c>
+      <c r="BT50" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU50" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, directly addressing the prompt without any ambiguity.</t>
+        </is>
+      </c>
+      <c r="BV50" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW50" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by clarifying the lack of gender in a language model.</t>
+        </is>
+      </c>
+      <c r="BX50" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY50" t="inlineStr">
+        <is>
+          <t>The response perfectly adheres to the prompt by clearly stating that the entity does not have a gender and is not male or female.</t>
+        </is>
+      </c>
+      <c r="BZ50" t="n">
+        <v>8</v>
+      </c>
+      <c r="CA50" t="inlineStr">
+        <is>
+          <t>The response effectively highlights the distinction between human qualities and the neutral nature of a language model, providing a clear and insightful understanding of the technology.</t>
+        </is>
+      </c>
+      <c r="CB50" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC50" t="inlineStr">
+        <is>
+          <t>The two responses convey the same core meaning that the entity does not have a gender, but Message A provides additional detail about being a language model.</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -12033,6 +14445,54 @@
       <c r="BO51" t="inlineStr"/>
       <c r="BP51" t="inlineStr"/>
       <c r="BQ51" t="inlineStr"/>
+      <c r="BR51" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS51" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Mount Everest as the tallest mountain in the world and provides the accurate height.</t>
+        </is>
+      </c>
+      <c r="BT51" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU51" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, providing both the name of the mountain and its exact height in two different units.</t>
+        </is>
+      </c>
+      <c r="BV51" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW51" t="inlineStr">
+        <is>
+          <t>The response directly and accurately answers the prompt by identifying Mount Everest as the tallest mountain in the world and providing its height.</t>
+        </is>
+      </c>
+      <c r="BX51" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY51" t="inlineStr">
+        <is>
+          <t>The response directly and accurately answers the prompt, providing the name and height of the tallest mountain in the world.</t>
+        </is>
+      </c>
+      <c r="BZ51" t="n">
+        <v>5</v>
+      </c>
+      <c r="CA51" t="inlineStr">
+        <is>
+          <t>The response accurately identifies Mount Everest as the tallest mountain but offers minimal additional insight beyond basic facts.</t>
+        </is>
+      </c>
+      <c r="CB51" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC51" t="inlineStr">
+        <is>
+          <t>While Message A provides additional details about the height of Mount Everest, the core substance and meaning are the same as in Message B, identifying Mount Everest as the tallest mountain in the world.</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -12232,6 +14692,54 @@
       <c r="BO52" t="inlineStr"/>
       <c r="BP52" t="inlineStr"/>
       <c r="BQ52" t="inlineStr"/>
+      <c r="BR52" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS52" t="inlineStr">
+        <is>
+          <t>The response correctly identifies the boiling point of water as 100 degrees Celsius (212 degrees Fahrenheit) and accurately explains the condition for boiling.</t>
+        </is>
+      </c>
+      <c r="BT52" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU52" t="inlineStr">
+        <is>
+          <t>The response is clear, concise, and easy to understand, providing both the boiling point in Celsius and Fahrenheit along with a brief explanation.</t>
+        </is>
+      </c>
+      <c r="BV52" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW52" t="inlineStr">
+        <is>
+          <t>The response directly and accurately addresses the prompt by providing the boiling point of water in both Celsius and Fahrenheit, along with a relevant explanation.</t>
+        </is>
+      </c>
+      <c r="BX52" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY52" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by providing the boiling point of water in both Celsius and Fahrenheit, although it includes a minor additional explanation that slightly exceeds the prompt's core request.</t>
+        </is>
+      </c>
+      <c r="BZ52" t="n">
+        <v>5</v>
+      </c>
+      <c r="CA52" t="inlineStr">
+        <is>
+          <t>The response provides accurate and relevant information about the boiling point of water but lacks any additional insight or deeper exploration of the topic.</t>
+        </is>
+      </c>
+      <c r="CB52" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC52" t="inlineStr">
+        <is>
+          <t>While Message A provides additional explanatory details about the boiling point, both messages convey the same fundamental information about the boiling point of water being 100°C or 212°F.</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -12432,6 +14940,54 @@
       <c r="BO53" t="inlineStr"/>
       <c r="BP53" t="inlineStr"/>
       <c r="BQ53" t="inlineStr"/>
+      <c r="BR53" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS53" t="inlineStr">
+        <is>
+          <t>The response is completely factually correct as there are indeed 7 days in a week.</t>
+        </is>
+      </c>
+      <c r="BT53" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU53" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, providing a direct and accurate answer to the prompt.</t>
+        </is>
+      </c>
+      <c r="BV53" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW53" t="inlineStr">
+        <is>
+          <t>The response directly and accurately answers the prompt with no irrelevant information.</t>
+        </is>
+      </c>
+      <c r="BX53" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY53" t="inlineStr">
+        <is>
+          <t>The response directly answers the prompt's question but includes additional information that, while relevant, goes slightly beyond what was asked.</t>
+        </is>
+      </c>
+      <c r="BZ53" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA53" t="inlineStr">
+        <is>
+          <t>The response merely states a widely known fact without providing any additional depth or perspective.</t>
+        </is>
+      </c>
+      <c r="CB53" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC53" t="inlineStr">
+        <is>
+          <t>Message A provides additional context, but both messages convey the same core information that there are 7 days in a week.</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -12631,6 +15187,54 @@
       <c r="BO54" t="inlineStr"/>
       <c r="BP54" t="inlineStr"/>
       <c r="BQ54" t="inlineStr"/>
+      <c r="BR54" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS54" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Harper Lee as the author of 'To Kill a Mockingbird' and accurately describes the themes of her work, but it incorrectly states that she was born in New Orleans, Louisiana (she was born in Monroeville, Alabama), which slightly reduces the accuracy score.</t>
+        </is>
+      </c>
+      <c r="BT54" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU54" t="inlineStr">
+        <is>
+          <t>The response is clear, concise, and directly answers the prompt with additional relevant context about the author, Harper Lee, without any confusing or misleading information.</t>
+        </is>
+      </c>
+      <c r="BV54" t="n">
+        <v>7</v>
+      </c>
+      <c r="BW54" t="inlineStr">
+        <is>
+          <t>The response directly answers the prompt by identifying Harper Lee as the author of 'To Kill a Mockingbird' but also includes additional biographical and thematic information that is less relevant to the specific question asked.</t>
+        </is>
+      </c>
+      <c r="BX54" t="n">
+        <v>7</v>
+      </c>
+      <c r="BY54" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Harper Lee as the author of 'To Kill a Mockingbird' but includes additional biographical information that goes beyond the prompt's specific question.</t>
+        </is>
+      </c>
+      <c r="BZ54" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA54" t="inlineStr">
+        <is>
+          <t>The response provides some insight into Harper Lee's background and the themes of her work, but it lacks deeper analysis or original thought that would make it highly insightful.</t>
+        </is>
+      </c>
+      <c r="CB54" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC54" t="inlineStr">
+        <is>
+          <t>While Message A correctly identifies Harper Lee as the author of 'To Kill a Mockingbird', it includes additional biographical information and context that is not present in the concise benchmark response, resulting in some variance.</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -12831,6 +15435,54 @@
       <c r="BO55" t="inlineStr"/>
       <c r="BP55" t="inlineStr"/>
       <c r="BQ55" t="inlineStr"/>
+      <c r="BR55" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS55" t="inlineStr">
+        <is>
+          <t>The response correctly identifies the question and accurately provides the sum of 1+2 as 3.</t>
+        </is>
+      </c>
+      <c r="BT55" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU55" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, with a straightforward explanation and correct answer.</t>
+        </is>
+      </c>
+      <c r="BV55" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW55" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by providing the calculation and the correct answer.</t>
+        </is>
+      </c>
+      <c r="BX55" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY55" t="inlineStr">
+        <is>
+          <t>The response directly answers the prompt's question and provides the correct arithmetic solution.</t>
+        </is>
+      </c>
+      <c r="BZ55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA55" t="inlineStr">
+        <is>
+          <t>The response merely restates the question and provides the obvious calculation without offering any additional perspective or depth.</t>
+        </is>
+      </c>
+      <c r="CB55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC55" t="inlineStr">
+        <is>
+          <t>While both messages convey the correct result of the calculation, Message A includes additional explanatory text that is absent in the benchmark Message B.</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -13034,6 +15686,54 @@
       <c r="BO56" t="inlineStr"/>
       <c r="BP56" t="inlineStr"/>
       <c r="BQ56" t="inlineStr"/>
+      <c r="BR56" t="n">
+        <v>5</v>
+      </c>
+      <c r="BS56" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Christmas as a holiday celebrated by Christians but incorrectly states the duration, as Christmas is primarily celebrated on December 25th, with related celebrations varying in length and dates.</t>
+        </is>
+      </c>
+      <c r="BT56" t="n">
+        <v>7</v>
+      </c>
+      <c r="BU56" t="inlineStr">
+        <is>
+          <t>The response clearly identifies Christmas as a holiday and its general time frame, but the specific dates mentioned are not entirely accurate, causing some confusion.</t>
+        </is>
+      </c>
+      <c r="BV56" t="n">
+        <v>8</v>
+      </c>
+      <c r="BW56" t="inlineStr">
+        <is>
+          <t>The response provides relevant information about the date Christmas is celebrated but includes some additional context that is not directly asked for in the prompt.</t>
+        </is>
+      </c>
+      <c r="BX56" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY56" t="inlineStr">
+        <is>
+          <t>The response provides relevant information about Christmas, including the date, but slightly deviates by mentioning the duration of the celebration instead of sticking to a single date.</t>
+        </is>
+      </c>
+      <c r="BZ56" t="n">
+        <v>3</v>
+      </c>
+      <c r="CA56" t="inlineStr">
+        <is>
+          <t>The response provides basic factual information about Christmas but lacks depth or original insight into the holiday's significance or cultural nuances.</t>
+        </is>
+      </c>
+      <c r="CB56" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC56" t="inlineStr">
+        <is>
+          <t>Message A provides additional context about Christmas and a date range, while Message B only gives the specific date, leading to a moderate variance in substance and meaning.</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -13233,6 +15933,54 @@
       <c r="BO57" t="inlineStr"/>
       <c r="BP57" t="inlineStr"/>
       <c r="BQ57" t="inlineStr"/>
+      <c r="BR57" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS57" t="inlineStr">
+        <is>
+          <t>The response correctly identifies the speaker as an artificial intelligence without gender, which is entirely factually accurate.</t>
+        </is>
+      </c>
+      <c r="BT57" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU57" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, explicitly stating that the entity is an artificial intelligence without a gender.</t>
+        </is>
+      </c>
+      <c r="BV57" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW57" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt by clearly stating the lack of gender as an artificial intelligence.</t>
+        </is>
+      </c>
+      <c r="BX57" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY57" t="inlineStr">
+        <is>
+          <t>The response directly addresses the prompt about gender but goes slightly beyond by mentioning its nature as an artificial intelligence, which is still relevant.</t>
+        </is>
+      </c>
+      <c r="BZ57" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA57" t="inlineStr">
+        <is>
+          <t>The response concisely and clearly explains the nature of artificial intelligence, demonstrating an understanding of the prompt and providing a thoughtful answer.</t>
+        </is>
+      </c>
+      <c r="CB57" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC57" t="inlineStr">
+        <is>
+          <t>Message A provides more detail but the core meaning and substance are very similar to Message B.</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -13433,6 +16181,54 @@
       <c r="BO58" t="inlineStr"/>
       <c r="BP58" t="inlineStr"/>
       <c r="BQ58" t="inlineStr"/>
+      <c r="BR58" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS58" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Paris as the capital of France, which is entirely accurate.</t>
+        </is>
+      </c>
+      <c r="BT58" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU58" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand. It directly answers the prompt with precise and accurate information.</t>
+        </is>
+      </c>
+      <c r="BV58" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW58" t="inlineStr">
+        <is>
+          <t>The response directly and accurately answers the prompt, providing the capital of France.</t>
+        </is>
+      </c>
+      <c r="BX58" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY58" t="inlineStr">
+        <is>
+          <t>The response perfectly adheres to the prompt by providing the correct and direct answer.</t>
+        </is>
+      </c>
+      <c r="BZ58" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA58" t="inlineStr">
+        <is>
+          <t>The response is factually correct but lacks any originality, depth, or additional insight, making it rather basic and uninspired.</t>
+        </is>
+      </c>
+      <c r="CB58" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC58" t="inlineStr">
+        <is>
+          <t>The two messages convey essentially the same information, with Message A providing slightly more detail but no significant difference in substance or meaning.</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -13632,6 +16428,54 @@
       <c r="BO59" t="inlineStr"/>
       <c r="BP59" t="inlineStr"/>
       <c r="BQ59" t="inlineStr"/>
+      <c r="BR59" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS59" t="inlineStr">
+        <is>
+          <t>The response correctly states that there are 7 days in a week, which is factually accurate.</t>
+        </is>
+      </c>
+      <c r="BT59" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU59" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, explicitly stating the number of days in a week.</t>
+        </is>
+      </c>
+      <c r="BV59" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW59" t="inlineStr">
+        <is>
+          <t>The response directly answers the prompt by stating there are 7 days in a week and elaborates correctly on the concept of a week.</t>
+        </is>
+      </c>
+      <c r="BX59" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY59" t="inlineStr">
+        <is>
+          <t>The response accurately answers the prompt but includes a minor additional detail that was not asked for.</t>
+        </is>
+      </c>
+      <c r="BZ59" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA59" t="inlineStr">
+        <is>
+          <t>The response merely states a well-known fact without offering any additional perspective or depth.</t>
+        </is>
+      </c>
+      <c r="CB59" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC59" t="inlineStr">
+        <is>
+          <t>While Message A includes additional explanatory details, both messages correctly identify the number of days in a week as 7, resulting in low variance.</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -13831,6 +16675,54 @@
       <c r="BO60" t="inlineStr"/>
       <c r="BP60" t="inlineStr"/>
       <c r="BQ60" t="inlineStr"/>
+      <c r="BR60" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS60" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Jupiter as the largest planet in our solar system and provides accurate data regarding its mass, diameter, and volume.</t>
+        </is>
+      </c>
+      <c r="BT60" t="n">
+        <v>10</v>
+      </c>
+      <c r="BU60" t="inlineStr">
+        <is>
+          <t>The response is perfectly clear and easy to understand, providing precise and relevant information about the largest planet in our solar system.</t>
+        </is>
+      </c>
+      <c r="BV60" t="n">
+        <v>10</v>
+      </c>
+      <c r="BW60" t="inlineStr">
+        <is>
+          <t>The response directly and accurately answers the prompt about the largest planet in our solar system, providing additional relevant details about Jupiter.</t>
+        </is>
+      </c>
+      <c r="BX60" t="n">
+        <v>8</v>
+      </c>
+      <c r="BY60" t="inlineStr">
+        <is>
+          <t>The response correctly identifies Jupiter as the largest planet but includes additional details that go beyond the prompt's simple question.</t>
+        </is>
+      </c>
+      <c r="BZ60" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA60" t="inlineStr">
+        <is>
+          <t>While the response accurately identifies Jupiter as the largest planet and provides relevant data, it lacks deeper analysis or unique perspective that would make it highly insightful.</t>
+        </is>
+      </c>
+      <c r="CB60" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC60" t="inlineStr">
+        <is>
+          <t>While Message A provides additional details about Jupiter, it accurately identifies Jupiter as the largest planet in our solar system, aligning with the substance and meaning of Message B.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>